<commit_message>
Modified dummy data for fact customer metrics
</commit_message>
<xml_diff>
--- a/Dummy Data/Fact_Customer_Metrics.xlsx
+++ b/Dummy Data/Fact_Customer_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COLLEGE\BITS PILANI\SS 2nd Semester\DW\DW Project\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344E24FA-8A50-44B5-AC30-6EBCC2A6CB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C7DE6B-A753-4557-89A8-FF69F37B0553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="N198" sqref="N198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,7 +375,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>20110101</v>
@@ -386,563 +386,563 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>20110201</v>
+        <v>20110101</v>
       </c>
       <c r="C3">
-        <v>694</v>
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>20110301</v>
+        <v>20110101</v>
       </c>
       <c r="C4">
-        <v>730</v>
+        <v>788</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>20110401</v>
+        <v>20110201</v>
       </c>
       <c r="C5">
-        <v>683</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>20110501</v>
+        <v>20110201</v>
       </c>
       <c r="C6">
-        <v>709</v>
+        <v>694</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B7">
-        <v>20110601</v>
+        <v>20110201</v>
       </c>
       <c r="C7">
-        <v>815</v>
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>20110701</v>
+        <v>20110301</v>
       </c>
       <c r="C8">
-        <v>323</v>
+        <v>730</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B9">
-        <v>20110801</v>
+        <v>20110301</v>
       </c>
       <c r="C9">
-        <v>427</v>
+        <v>730</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>20110901</v>
+        <v>20110301</v>
       </c>
       <c r="C10">
-        <v>356</v>
+        <v>700</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>20111001</v>
+        <v>20110401</v>
       </c>
       <c r="C11">
-        <v>696</v>
+        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B12">
-        <v>20111101</v>
+        <v>20110401</v>
       </c>
       <c r="C12">
-        <v>520</v>
+        <v>683</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>20111201</v>
+        <v>20110401</v>
       </c>
       <c r="C13">
-        <v>766</v>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>20120101</v>
+        <v>20110501</v>
       </c>
       <c r="C14">
-        <v>741</v>
+        <v>709</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>20120201</v>
+        <v>20110501</v>
       </c>
       <c r="C15">
-        <v>785</v>
+        <v>709</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B16">
-        <v>20120301</v>
+        <v>20110501</v>
       </c>
       <c r="C16">
-        <v>703</v>
+        <v>687</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>20120401</v>
+        <v>20110601</v>
       </c>
       <c r="C17">
-        <v>711</v>
+        <v>815</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B18">
-        <v>20120501</v>
+        <v>20110601</v>
       </c>
       <c r="C18">
-        <v>706</v>
+        <v>815</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B19">
-        <v>20120601</v>
+        <v>20110601</v>
       </c>
       <c r="C19">
-        <v>737</v>
+        <v>848</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>20120701</v>
+        <v>20110701</v>
       </c>
       <c r="C20">
-        <v>753</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>20120801</v>
+        <v>20110701</v>
       </c>
       <c r="C21">
-        <v>541</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22">
-        <v>20120901</v>
+        <v>20110701</v>
       </c>
       <c r="C22">
-        <v>728</v>
+        <v>786</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23">
-        <v>20121001</v>
+        <v>20110801</v>
       </c>
       <c r="C23">
-        <v>680</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>20121101</v>
+        <v>20110801</v>
       </c>
       <c r="C24">
-        <v>818</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>20121201</v>
+        <v>20110801</v>
       </c>
       <c r="C25">
-        <v>690</v>
+        <v>681</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>20130101</v>
+        <v>20110901</v>
       </c>
       <c r="C26">
-        <v>674</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B27">
-        <v>20130201</v>
+        <v>20110901</v>
       </c>
       <c r="C27">
-        <v>714</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>20130301</v>
+        <v>20110901</v>
       </c>
       <c r="C28">
-        <v>727</v>
+        <v>694</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>20130401</v>
+        <v>20111001</v>
       </c>
       <c r="C29">
-        <v>310</v>
+        <v>696</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>20130501</v>
+        <v>20111001</v>
       </c>
       <c r="C30">
-        <v>392</v>
+        <v>696</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>20130601</v>
+        <v>20111001</v>
       </c>
       <c r="C31">
-        <v>716</v>
+        <v>680</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B32">
-        <v>20130701</v>
+        <v>20111101</v>
       </c>
       <c r="C32">
-        <v>407</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33">
-        <v>20130801</v>
+        <v>20111101</v>
       </c>
       <c r="C33">
-        <v>736</v>
+        <v>520</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B34">
-        <v>20130901</v>
+        <v>20111101</v>
       </c>
       <c r="C34">
-        <v>696</v>
+        <v>738</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B35">
-        <v>20131001</v>
+        <v>20111201</v>
       </c>
       <c r="C35">
-        <v>717</v>
+        <v>766</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B36">
-        <v>20131101</v>
+        <v>20111201</v>
       </c>
       <c r="C36">
-        <v>799</v>
+        <v>766</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37">
-        <v>20131201</v>
+        <v>20111201</v>
       </c>
       <c r="C37">
-        <v>804</v>
+        <v>709</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B38">
-        <v>20140101</v>
+        <v>20120101</v>
       </c>
       <c r="C38">
-        <v>736</v>
+        <v>741</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39">
-        <v>20140201</v>
+        <v>20120101</v>
       </c>
       <c r="C39">
-        <v>681</v>
+        <v>741</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40">
-        <v>20140301</v>
+        <v>20120101</v>
       </c>
       <c r="C40">
-        <v>355</v>
+        <v>711</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B41">
-        <v>20140401</v>
+        <v>20120201</v>
       </c>
       <c r="C41">
-        <v>721</v>
+        <v>785</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B42">
-        <v>20140501</v>
+        <v>20120201</v>
       </c>
       <c r="C42">
-        <v>735</v>
+        <v>698</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B43">
-        <v>20140601</v>
+        <v>20120201</v>
       </c>
       <c r="C43">
-        <v>712</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44">
-        <v>20140701</v>
+        <v>20120301</v>
       </c>
       <c r="C44">
-        <v>885</v>
+        <v>703</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B45">
-        <v>20140801</v>
+        <v>20120301</v>
       </c>
       <c r="C45">
-        <v>870</v>
+        <v>694</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46">
-        <v>20140901</v>
+        <v>20120301</v>
       </c>
       <c r="C46">
-        <v>443</v>
+        <v>856</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B47">
-        <v>20141001</v>
+        <v>20120401</v>
       </c>
       <c r="C47">
-        <v>580</v>
+        <v>711</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B48">
-        <v>20141101</v>
+        <v>20120401</v>
       </c>
       <c r="C48">
-        <v>859</v>
+        <v>730</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B49">
-        <v>20141201</v>
+        <v>20120401</v>
       </c>
       <c r="C49">
-        <v>713</v>
+        <v>606</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B50">
-        <v>20150101</v>
+        <v>20120501</v>
       </c>
       <c r="C50">
-        <v>733</v>
+        <v>706</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="B51">
-        <v>20150201</v>
+        <v>20120501</v>
       </c>
       <c r="C51">
-        <v>503</v>
+        <v>683</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B52">
-        <v>20150301</v>
+        <v>20120501</v>
       </c>
       <c r="C52">
-        <v>699</v>
+        <v>789</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B53">
-        <v>20150401</v>
+        <v>20120601</v>
       </c>
       <c r="C53">
-        <v>462</v>
+        <v>737</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,513 +950,513 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>20150501</v>
+        <v>20120601</v>
       </c>
       <c r="C54">
-        <v>744</v>
+        <v>709</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="B55">
-        <v>20150601</v>
+        <v>20120601</v>
       </c>
       <c r="C55">
-        <v>884</v>
+        <v>759</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B56">
-        <v>20150701</v>
+        <v>20120701</v>
       </c>
       <c r="C56">
-        <v>723</v>
+        <v>753</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B57">
-        <v>20150801</v>
+        <v>20120701</v>
       </c>
       <c r="C57">
-        <v>379</v>
+        <v>815</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B58">
-        <v>20150901</v>
+        <v>20120701</v>
       </c>
       <c r="C58">
-        <v>722</v>
+        <v>731</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B59">
-        <v>20151001</v>
+        <v>20120801</v>
       </c>
       <c r="C59">
-        <v>703</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="B60">
-        <v>20151101</v>
+        <v>20120801</v>
       </c>
       <c r="C60">
-        <v>696</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61">
-        <v>20151201</v>
+        <v>20120801</v>
       </c>
       <c r="C61">
-        <v>456</v>
+        <v>796</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B62">
-        <v>20160101</v>
+        <v>20120901</v>
       </c>
       <c r="C62">
-        <v>466</v>
+        <v>728</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B63">
-        <v>20160201</v>
+        <v>20120901</v>
       </c>
       <c r="C63">
-        <v>733</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B64">
-        <v>20160301</v>
+        <v>20120901</v>
       </c>
       <c r="C64">
-        <v>665</v>
+        <v>559</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B65">
-        <v>20160401</v>
+        <v>20121001</v>
       </c>
       <c r="C65">
-        <v>412</v>
+        <v>680</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B66">
-        <v>20160501</v>
+        <v>20121001</v>
       </c>
       <c r="C66">
-        <v>542</v>
+        <v>356</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B67">
-        <v>20160601</v>
+        <v>20121001</v>
       </c>
       <c r="C67">
-        <v>705</v>
+        <v>721</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B68">
-        <v>20160701</v>
+        <v>20121101</v>
       </c>
       <c r="C68">
-        <v>788</v>
+        <v>818</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="B69">
-        <v>20160801</v>
+        <v>20121101</v>
       </c>
       <c r="C69">
-        <v>708</v>
+        <v>696</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B70">
-        <v>20160901</v>
+        <v>20121101</v>
       </c>
       <c r="C70">
-        <v>700</v>
+        <v>762</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B71">
-        <v>20161001</v>
+        <v>20121201</v>
       </c>
       <c r="C71">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B72">
-        <v>20161101</v>
+        <v>20121201</v>
       </c>
       <c r="C72">
-        <v>687</v>
+        <v>520</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B73">
-        <v>20161201</v>
+        <v>20121201</v>
       </c>
       <c r="C73">
-        <v>848</v>
+        <v>513</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B74">
-        <v>20170101</v>
+        <v>20130101</v>
       </c>
       <c r="C74">
-        <v>786</v>
+        <v>674</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B75">
-        <v>20170201</v>
+        <v>20130101</v>
       </c>
       <c r="C75">
-        <v>681</v>
+        <v>766</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="B76">
-        <v>20170301</v>
+        <v>20130101</v>
       </c>
       <c r="C76">
-        <v>694</v>
+        <v>733</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="B77">
-        <v>20170401</v>
+        <v>20130201</v>
       </c>
       <c r="C77">
-        <v>680</v>
+        <v>714</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="B78">
-        <v>20170501</v>
+        <v>20130201</v>
       </c>
       <c r="C78">
-        <v>738</v>
+        <v>741</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B79">
-        <v>20170601</v>
+        <v>20130201</v>
       </c>
       <c r="C79">
-        <v>709</v>
+        <v>735</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B80">
-        <v>20170701</v>
+        <v>20130301</v>
       </c>
       <c r="C80">
-        <v>711</v>
+        <v>727</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="B81">
-        <v>20170801</v>
+        <v>20130301</v>
       </c>
       <c r="C81">
-        <v>304</v>
+        <v>785</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="B82">
-        <v>20170901</v>
+        <v>20130301</v>
       </c>
       <c r="C82">
-        <v>856</v>
+        <v>707</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B83">
-        <v>20171001</v>
+        <v>20130401</v>
       </c>
       <c r="C83">
-        <v>606</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B84">
-        <v>20171101</v>
+        <v>20130401</v>
       </c>
       <c r="C84">
-        <v>789</v>
+        <v>703</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="B85">
-        <v>20171201</v>
+        <v>20130401</v>
       </c>
       <c r="C85">
-        <v>759</v>
+        <v>845</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="B86">
-        <v>20180101</v>
+        <v>20130501</v>
       </c>
       <c r="C86">
-        <v>731</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="B87">
-        <v>20180201</v>
+        <v>20130501</v>
       </c>
       <c r="C87">
-        <v>796</v>
+        <v>711</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B88">
-        <v>20180301</v>
+        <v>20130501</v>
       </c>
       <c r="C88">
-        <v>559</v>
+        <v>657</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="B89">
-        <v>20180401</v>
+        <v>20130601</v>
       </c>
       <c r="C89">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="B90">
-        <v>20180501</v>
+        <v>20130601</v>
       </c>
       <c r="C90">
-        <v>762</v>
+        <v>706</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B91">
-        <v>20180601</v>
+        <v>20130601</v>
       </c>
       <c r="C91">
-        <v>513</v>
+        <v>703</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B92">
-        <v>20180701</v>
+        <v>20130701</v>
       </c>
       <c r="C92">
-        <v>733</v>
+        <v>407</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B93">
-        <v>20180801</v>
+        <v>20130701</v>
       </c>
       <c r="C93">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="B94">
-        <v>20180901</v>
+        <v>20130701</v>
       </c>
       <c r="C94">
-        <v>707</v>
+        <v>525</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="B95">
-        <v>20181001</v>
+        <v>20130801</v>
       </c>
       <c r="C95">
-        <v>845</v>
+        <v>736</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="B96">
-        <v>20181101</v>
+        <v>20130801</v>
       </c>
       <c r="C96">
-        <v>657</v>
+        <v>753</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="B97">
-        <v>20181201</v>
+        <v>20130801</v>
       </c>
       <c r="C97">
-        <v>703</v>
+        <v>724</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="B98">
-        <v>20190101</v>
+        <v>20130901</v>
       </c>
       <c r="C98">
-        <v>525</v>
+        <v>696</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B99">
-        <v>20190201</v>
+        <v>20130901</v>
       </c>
       <c r="C99">
-        <v>724</v>
+        <v>541</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="B100">
-        <v>20190301</v>
+        <v>20130901</v>
       </c>
       <c r="C100">
         <v>721</v>
@@ -1464,236 +1464,2219 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="B101">
-        <v>20190401</v>
+        <v>20131001</v>
       </c>
       <c r="C101">
-        <v>534</v>
+        <v>717</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="B102">
-        <v>20190501</v>
+        <v>20131001</v>
       </c>
       <c r="C102">
-        <v>684</v>
+        <v>728</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="B103">
-        <v>20190601</v>
+        <v>20131001</v>
       </c>
       <c r="C103">
-        <v>784</v>
+        <v>534</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="B104">
-        <v>20190701</v>
+        <v>20131101</v>
       </c>
       <c r="C104">
-        <v>723</v>
+        <v>799</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="B105">
-        <v>20190801</v>
+        <v>20131101</v>
       </c>
       <c r="C105">
-        <v>638</v>
+        <v>680</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="B106">
-        <v>20190901</v>
+        <v>20131101</v>
       </c>
       <c r="C106">
-        <v>751</v>
+        <v>684</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="B107">
-        <v>20191001</v>
+        <v>20131201</v>
       </c>
       <c r="C107">
-        <v>715</v>
+        <v>804</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="B108">
-        <v>20191101</v>
+        <v>20131201</v>
       </c>
       <c r="C108">
-        <v>688</v>
+        <v>818</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="B109">
-        <v>20191201</v>
+        <v>20131201</v>
       </c>
       <c r="C109">
-        <v>727</v>
+        <v>784</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="B110">
-        <v>20200101</v>
+        <v>20140101</v>
       </c>
       <c r="C110">
-        <v>726</v>
+        <v>736</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="B111">
-        <v>20200201</v>
+        <v>20140101</v>
       </c>
       <c r="C111">
-        <v>704</v>
+        <v>690</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="B112">
-        <v>20200301</v>
+        <v>20140101</v>
       </c>
       <c r="C112">
-        <v>883</v>
+        <v>723</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="B113">
-        <v>20200401</v>
+        <v>20140201</v>
       </c>
       <c r="C113">
-        <v>741</v>
+        <v>681</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="B114">
-        <v>20200501</v>
+        <v>20140201</v>
       </c>
       <c r="C114">
-        <v>703</v>
+        <v>674</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="B115">
-        <v>20200601</v>
+        <v>20140201</v>
       </c>
       <c r="C115">
-        <v>691</v>
+        <v>638</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="B116">
-        <v>20200701</v>
+        <v>20140301</v>
       </c>
       <c r="C116">
-        <v>688</v>
+        <v>355</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="B117">
-        <v>20200801</v>
+        <v>20140301</v>
       </c>
       <c r="C117">
-        <v>814</v>
+        <v>714</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="B118">
-        <v>20200901</v>
+        <v>20140301</v>
       </c>
       <c r="C118">
-        <v>866</v>
+        <v>751</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="B119">
-        <v>20201001</v>
+        <v>20140401</v>
       </c>
       <c r="C119">
-        <v>471</v>
+        <v>721</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="B120">
-        <v>20201101</v>
+        <v>20140401</v>
       </c>
       <c r="C120">
-        <v>696</v>
+        <v>727</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="B121">
+        <v>20140401</v>
+      </c>
+      <c r="C121">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>60</v>
+      </c>
+      <c r="B122">
+        <v>20140501</v>
+      </c>
+      <c r="C122">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>8</v>
+      </c>
+      <c r="B123">
+        <v>20140501</v>
+      </c>
+      <c r="C123">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>28</v>
+      </c>
+      <c r="B124">
+        <v>20140501</v>
+      </c>
+      <c r="C124">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>13</v>
+      </c>
+      <c r="B125">
+        <v>20140601</v>
+      </c>
+      <c r="C125">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>60</v>
+      </c>
+      <c r="B126">
+        <v>20140601</v>
+      </c>
+      <c r="C126">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>33</v>
+      </c>
+      <c r="B127">
+        <v>20140601</v>
+      </c>
+      <c r="C127">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>6</v>
+      </c>
+      <c r="B128">
+        <v>20140701</v>
+      </c>
+      <c r="C128">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>26</v>
+      </c>
+      <c r="B129">
+        <v>20140701</v>
+      </c>
+      <c r="C129">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>10</v>
+      </c>
+      <c r="B130">
+        <v>20140701</v>
+      </c>
+      <c r="C130">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>38</v>
+      </c>
+      <c r="B131">
+        <v>20140801</v>
+      </c>
+      <c r="C131">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>25</v>
+      </c>
+      <c r="B132">
+        <v>20140801</v>
+      </c>
+      <c r="C132">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>59</v>
+      </c>
+      <c r="B133">
+        <v>20140801</v>
+      </c>
+      <c r="C133">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>49</v>
+      </c>
+      <c r="B134">
+        <v>20140901</v>
+      </c>
+      <c r="C134">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>47</v>
+      </c>
+      <c r="B135">
+        <v>20140901</v>
+      </c>
+      <c r="C135">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>3</v>
+      </c>
+      <c r="B136">
+        <v>20140901</v>
+      </c>
+      <c r="C136">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>4</v>
+      </c>
+      <c r="B137">
+        <v>20141001</v>
+      </c>
+      <c r="C137">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1</v>
+      </c>
+      <c r="B138">
+        <v>20141001</v>
+      </c>
+      <c r="C138">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>5</v>
+      </c>
+      <c r="B139">
+        <v>20141001</v>
+      </c>
+      <c r="C139">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>55</v>
+      </c>
+      <c r="B140">
+        <v>20141101</v>
+      </c>
+      <c r="C140">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>52</v>
+      </c>
+      <c r="B141">
+        <v>20141101</v>
+      </c>
+      <c r="C141">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>22</v>
+      </c>
+      <c r="B142">
+        <v>20141101</v>
+      </c>
+      <c r="C142">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>60</v>
+      </c>
+      <c r="B143">
+        <v>20141201</v>
+      </c>
+      <c r="C143">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>47</v>
+      </c>
+      <c r="B144">
+        <v>20141201</v>
+      </c>
+      <c r="C144">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>2</v>
+      </c>
+      <c r="B145">
+        <v>20141201</v>
+      </c>
+      <c r="C145">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>39</v>
+      </c>
+      <c r="B146">
+        <v>20150101</v>
+      </c>
+      <c r="C146">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>12</v>
+      </c>
+      <c r="B147">
+        <v>20150101</v>
+      </c>
+      <c r="C147">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>29</v>
+      </c>
+      <c r="B148">
+        <v>20150101</v>
+      </c>
+      <c r="C148">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>50</v>
+      </c>
+      <c r="B149">
+        <v>20150201</v>
+      </c>
+      <c r="C149">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>6</v>
+      </c>
+      <c r="B150">
+        <v>20150201</v>
+      </c>
+      <c r="C150">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>45</v>
+      </c>
+      <c r="B151">
+        <v>20150201</v>
+      </c>
+      <c r="C151">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>20150301</v>
+      </c>
+      <c r="C152">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>59</v>
+      </c>
+      <c r="B153">
+        <v>20150301</v>
+      </c>
+      <c r="C153">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>41</v>
+      </c>
+      <c r="B154">
+        <v>20150301</v>
+      </c>
+      <c r="C154">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>25</v>
+      </c>
+      <c r="B155">
+        <v>20150401</v>
+      </c>
+      <c r="C155">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>35</v>
+      </c>
+      <c r="B156">
+        <v>20150401</v>
+      </c>
+      <c r="C156">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>56</v>
+      </c>
+      <c r="B157">
+        <v>20150401</v>
+      </c>
+      <c r="C157">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>47</v>
+      </c>
+      <c r="B158">
+        <v>20150501</v>
+      </c>
+      <c r="C158">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>18</v>
+      </c>
+      <c r="B159">
+        <v>20150501</v>
+      </c>
+      <c r="C159">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>47</v>
+      </c>
+      <c r="B160">
+        <v>20150501</v>
+      </c>
+      <c r="C160">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>43</v>
+      </c>
+      <c r="B161">
+        <v>20150601</v>
+      </c>
+      <c r="C161">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>40</v>
+      </c>
+      <c r="B162">
+        <v>20150601</v>
+      </c>
+      <c r="C162">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>12</v>
+      </c>
+      <c r="B163">
+        <v>20150601</v>
+      </c>
+      <c r="C163">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>42</v>
+      </c>
+      <c r="B164">
+        <v>20150701</v>
+      </c>
+      <c r="C164">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>39</v>
+      </c>
+      <c r="B165">
+        <v>20150701</v>
+      </c>
+      <c r="C165">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>37</v>
+      </c>
+      <c r="B166">
+        <v>20150701</v>
+      </c>
+      <c r="C166">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>19</v>
+      </c>
+      <c r="B167">
+        <v>20150801</v>
+      </c>
+      <c r="C167">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>11</v>
+      </c>
+      <c r="B168">
+        <v>20150801</v>
+      </c>
+      <c r="C168">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>10</v>
+      </c>
+      <c r="B169">
+        <v>20150801</v>
+      </c>
+      <c r="C169">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>14</v>
+      </c>
+      <c r="B170">
+        <v>20150901</v>
+      </c>
+      <c r="C170">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>31</v>
+      </c>
+      <c r="B171">
+        <v>20150901</v>
+      </c>
+      <c r="C171">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>26</v>
+      </c>
+      <c r="B172">
+        <v>20150901</v>
+      </c>
+      <c r="C172">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>28</v>
+      </c>
+      <c r="B173">
+        <v>20151001</v>
+      </c>
+      <c r="C173">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>43</v>
+      </c>
+      <c r="B174">
+        <v>20151001</v>
+      </c>
+      <c r="C174">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>55</v>
+      </c>
+      <c r="B175">
+        <v>20151001</v>
+      </c>
+      <c r="C175">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>33</v>
+      </c>
+      <c r="B176">
+        <v>20151101</v>
+      </c>
+      <c r="C176">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>6</v>
+      </c>
+      <c r="B177">
+        <v>20151101</v>
+      </c>
+      <c r="C177">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>20151101</v>
+      </c>
+      <c r="C178">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>37</v>
+      </c>
+      <c r="B179">
+        <v>20151201</v>
+      </c>
+      <c r="C179">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>49</v>
+      </c>
+      <c r="B180">
+        <v>20151201</v>
+      </c>
+      <c r="C180">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>43</v>
+      </c>
+      <c r="B181">
+        <v>20151201</v>
+      </c>
+      <c r="C181">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>16</v>
+      </c>
+      <c r="B182">
+        <v>20160101</v>
+      </c>
+      <c r="C182">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>32</v>
+      </c>
+      <c r="B183">
+        <v>20160101</v>
+      </c>
+      <c r="C183">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>44</v>
+      </c>
+      <c r="B184">
+        <v>20160201</v>
+      </c>
+      <c r="C184">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>9</v>
+      </c>
+      <c r="B185">
+        <v>20160201</v>
+      </c>
+      <c r="C185">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>21</v>
+      </c>
+      <c r="B186">
+        <v>20160301</v>
+      </c>
+      <c r="C186">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>30</v>
+      </c>
+      <c r="B187">
+        <v>20160301</v>
+      </c>
+      <c r="C187">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>58</v>
+      </c>
+      <c r="B188">
+        <v>20160401</v>
+      </c>
+      <c r="C188">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>21</v>
+      </c>
+      <c r="B189">
+        <v>20160401</v>
+      </c>
+      <c r="C189">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2</v>
+      </c>
+      <c r="B190">
+        <v>20160501</v>
+      </c>
+      <c r="C190">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>57</v>
+      </c>
+      <c r="B191">
+        <v>20160501</v>
+      </c>
+      <c r="C191">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>29</v>
+      </c>
+      <c r="B192">
+        <v>20160601</v>
+      </c>
+      <c r="C192">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>18</v>
+      </c>
+      <c r="B193">
+        <v>20160601</v>
+      </c>
+      <c r="C193">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>49</v>
+      </c>
+      <c r="B194">
+        <v>20160701</v>
+      </c>
+      <c r="C194">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>27</v>
+      </c>
+      <c r="B195">
+        <v>20160701</v>
+      </c>
+      <c r="C195">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>24</v>
+      </c>
+      <c r="B196">
+        <v>20160801</v>
+      </c>
+      <c r="C196">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>56</v>
+      </c>
+      <c r="B197">
+        <v>20160801</v>
+      </c>
+      <c r="C197">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>32</v>
+      </c>
+      <c r="B198">
+        <v>20160901</v>
+      </c>
+      <c r="C198">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>4</v>
+      </c>
+      <c r="B199">
+        <v>20160901</v>
+      </c>
+      <c r="C199">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>58</v>
+      </c>
+      <c r="B200">
+        <v>20161001</v>
+      </c>
+      <c r="C200">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>21</v>
+      </c>
+      <c r="B201">
+        <v>20161001</v>
+      </c>
+      <c r="C201">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>12</v>
+      </c>
+      <c r="B202">
+        <v>20161101</v>
+      </c>
+      <c r="C202">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>30</v>
+      </c>
+      <c r="B203">
+        <v>20161101</v>
+      </c>
+      <c r="C203">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>5</v>
+      </c>
+      <c r="B204">
+        <v>20161201</v>
+      </c>
+      <c r="C204">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>21</v>
+      </c>
+      <c r="B205">
+        <v>20161201</v>
+      </c>
+      <c r="C205">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>57</v>
+      </c>
+      <c r="B206">
+        <v>20170101</v>
+      </c>
+      <c r="C206">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>24</v>
+      </c>
+      <c r="B207">
+        <v>20170101</v>
+      </c>
+      <c r="C207">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>20170201</v>
+      </c>
+      <c r="C208">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>45</v>
+      </c>
+      <c r="B209">
+        <v>20170201</v>
+      </c>
+      <c r="C209">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>34</v>
+      </c>
+      <c r="B210">
+        <v>20170301</v>
+      </c>
+      <c r="C210">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>33</v>
+      </c>
+      <c r="B211">
+        <v>20170301</v>
+      </c>
+      <c r="C211">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>36</v>
+      </c>
+      <c r="B212">
+        <v>20170401</v>
+      </c>
+      <c r="C212">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>24</v>
+      </c>
+      <c r="B213">
+        <v>20170401</v>
+      </c>
+      <c r="C213">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>29</v>
+      </c>
+      <c r="B214">
+        <v>20170501</v>
+      </c>
+      <c r="C214">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>46</v>
+      </c>
+      <c r="B215">
+        <v>20170501</v>
+      </c>
+      <c r="C215">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>49</v>
+      </c>
+      <c r="B216">
+        <v>20170601</v>
+      </c>
+      <c r="C216">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>41</v>
+      </c>
+      <c r="B217">
+        <v>20170601</v>
+      </c>
+      <c r="C217">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>4</v>
+      </c>
+      <c r="B218">
+        <v>20170701</v>
+      </c>
+      <c r="C218">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>30</v>
+      </c>
+      <c r="B219">
+        <v>20170701</v>
+      </c>
+      <c r="C219">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>25</v>
+      </c>
+      <c r="B220">
+        <v>20170801</v>
+      </c>
+      <c r="C220">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>18</v>
+      </c>
+      <c r="B221">
+        <v>20170801</v>
+      </c>
+      <c r="C221">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>3</v>
+      </c>
+      <c r="B222">
+        <v>20170901</v>
+      </c>
+      <c r="C222">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>30</v>
+      </c>
+      <c r="B223">
+        <v>20170901</v>
+      </c>
+      <c r="C223">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>14</v>
+      </c>
+      <c r="B224">
+        <v>20171001</v>
+      </c>
+      <c r="C224">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>14</v>
+      </c>
+      <c r="B225">
+        <v>20171001</v>
+      </c>
+      <c r="C225">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>50</v>
+      </c>
+      <c r="B226">
+        <v>20171101</v>
+      </c>
+      <c r="C226">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>34</v>
+      </c>
+      <c r="B227">
+        <v>20171101</v>
+      </c>
+      <c r="C227">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>51</v>
+      </c>
+      <c r="B228">
+        <v>20171201</v>
+      </c>
+      <c r="C228">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229">
+        <v>20171201</v>
+      </c>
+      <c r="C229">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>20</v>
+      </c>
+      <c r="B230">
+        <v>20180101</v>
+      </c>
+      <c r="C230">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>30</v>
+      </c>
+      <c r="B231">
+        <v>20180101</v>
+      </c>
+      <c r="C231">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>54</v>
+      </c>
+      <c r="B232">
+        <v>20180201</v>
+      </c>
+      <c r="C232">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>60</v>
+      </c>
+      <c r="B233">
+        <v>20180201</v>
+      </c>
+      <c r="C233">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>6</v>
+      </c>
+      <c r="B234">
+        <v>20180301</v>
+      </c>
+      <c r="C234">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>53</v>
+      </c>
+      <c r="B235">
+        <v>20180301</v>
+      </c>
+      <c r="C235">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>8</v>
+      </c>
+      <c r="B236">
+        <v>20180401</v>
+      </c>
+      <c r="C236">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>24</v>
+      </c>
+      <c r="B237">
+        <v>20180401</v>
+      </c>
+      <c r="C237">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>16</v>
+      </c>
+      <c r="B238">
+        <v>20180501</v>
+      </c>
+      <c r="C238">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>34</v>
+      </c>
+      <c r="B239">
+        <v>20180501</v>
+      </c>
+      <c r="C239">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>41</v>
+      </c>
+      <c r="B240">
+        <v>20180601</v>
+      </c>
+      <c r="C240">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>17</v>
+      </c>
+      <c r="B241">
+        <v>20180601</v>
+      </c>
+      <c r="C241">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>45</v>
+      </c>
+      <c r="B242">
+        <v>20180701</v>
+      </c>
+      <c r="C242">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>46</v>
+      </c>
+      <c r="B243">
+        <v>20180701</v>
+      </c>
+      <c r="C243">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>5</v>
+      </c>
+      <c r="B244">
+        <v>20180801</v>
+      </c>
+      <c r="C244">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>10</v>
+      </c>
+      <c r="B245">
+        <v>20180801</v>
+      </c>
+      <c r="C245">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>1</v>
+      </c>
+      <c r="B246">
+        <v>20180901</v>
+      </c>
+      <c r="C246">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>36</v>
+      </c>
+      <c r="B247">
+        <v>20180901</v>
+      </c>
+      <c r="C247">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>37</v>
+      </c>
+      <c r="B248">
+        <v>20181001</v>
+      </c>
+      <c r="C248">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>33</v>
+      </c>
+      <c r="B249">
+        <v>20181001</v>
+      </c>
+      <c r="C249">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>48</v>
+      </c>
+      <c r="B250">
+        <v>20181101</v>
+      </c>
+      <c r="C250">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>50</v>
+      </c>
+      <c r="B251">
+        <v>20181101</v>
+      </c>
+      <c r="C251">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>10</v>
+      </c>
+      <c r="B252">
+        <v>20181201</v>
+      </c>
+      <c r="C252">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>46</v>
+      </c>
+      <c r="B253">
+        <v>20181201</v>
+      </c>
+      <c r="C253">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>25</v>
+      </c>
+      <c r="B254">
+        <v>20190101</v>
+      </c>
+      <c r="C254">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>15</v>
+      </c>
+      <c r="B255">
+        <v>20190101</v>
+      </c>
+      <c r="C255">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>26</v>
+      </c>
+      <c r="B256">
+        <v>20190201</v>
+      </c>
+      <c r="C256">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>2</v>
+      </c>
+      <c r="B257">
+        <v>20190201</v>
+      </c>
+      <c r="C257">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>23</v>
+      </c>
+      <c r="B258">
+        <v>20190301</v>
+      </c>
+      <c r="C258">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>38</v>
+      </c>
+      <c r="B259">
+        <v>20190301</v>
+      </c>
+      <c r="C259">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>6</v>
+      </c>
+      <c r="B260">
+        <v>20190401</v>
+      </c>
+      <c r="C260">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>17</v>
+      </c>
+      <c r="B261">
+        <v>20190401</v>
+      </c>
+      <c r="C261">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>23</v>
+      </c>
+      <c r="B262">
+        <v>20190501</v>
+      </c>
+      <c r="C262">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>9</v>
+      </c>
+      <c r="B263">
+        <v>20190501</v>
+      </c>
+      <c r="C263">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>52</v>
+      </c>
+      <c r="B264">
+        <v>20190601</v>
+      </c>
+      <c r="C264">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>54</v>
+      </c>
+      <c r="B265">
+        <v>20190601</v>
+      </c>
+      <c r="C265">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>35</v>
+      </c>
+      <c r="B266">
+        <v>20190701</v>
+      </c>
+      <c r="C266">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>42</v>
+      </c>
+      <c r="B267">
+        <v>20190701</v>
+      </c>
+      <c r="C267">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>26</v>
+      </c>
+      <c r="B268">
+        <v>20190801</v>
+      </c>
+      <c r="C268">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>54</v>
+      </c>
+      <c r="B269">
+        <v>20190801</v>
+      </c>
+      <c r="C269">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>59</v>
+      </c>
+      <c r="B270">
+        <v>20190901</v>
+      </c>
+      <c r="C270">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>12</v>
+      </c>
+      <c r="B271">
+        <v>20190901</v>
+      </c>
+      <c r="C271">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>55</v>
+      </c>
+      <c r="B272">
+        <v>20191001</v>
+      </c>
+      <c r="C272">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>39</v>
+      </c>
+      <c r="B273">
+        <v>20191001</v>
+      </c>
+      <c r="C273">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>50</v>
+      </c>
+      <c r="B274">
+        <v>20191101</v>
+      </c>
+      <c r="C274">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>44</v>
+      </c>
+      <c r="B275">
+        <v>20191101</v>
+      </c>
+      <c r="C275">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>59</v>
+      </c>
+      <c r="B276">
+        <v>20191201</v>
+      </c>
+      <c r="C276">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>16</v>
+      </c>
+      <c r="B277">
+        <v>20191201</v>
+      </c>
+      <c r="C277">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>1</v>
+      </c>
+      <c r="B278">
+        <v>20200101</v>
+      </c>
+      <c r="C278">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>4</v>
+      </c>
+      <c r="B279">
+        <v>20200101</v>
+      </c>
+      <c r="C279">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>53</v>
+      </c>
+      <c r="B280">
+        <v>20200201</v>
+      </c>
+      <c r="C280">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>28</v>
+      </c>
+      <c r="B281">
+        <v>20200201</v>
+      </c>
+      <c r="C281">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>37</v>
+      </c>
+      <c r="B282">
+        <v>20200301</v>
+      </c>
+      <c r="C282">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>41</v>
+      </c>
+      <c r="B283">
+        <v>20200301</v>
+      </c>
+      <c r="C283">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>37</v>
+      </c>
+      <c r="B284">
+        <v>20200401</v>
+      </c>
+      <c r="C284">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>7</v>
+      </c>
+      <c r="B285">
+        <v>20200401</v>
+      </c>
+      <c r="C285">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>20</v>
+      </c>
+      <c r="B286">
+        <v>20200501</v>
+      </c>
+      <c r="C286">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>20</v>
+      </c>
+      <c r="B287">
+        <v>20200501</v>
+      </c>
+      <c r="C287">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>27</v>
+      </c>
+      <c r="B288">
+        <v>20200601</v>
+      </c>
+      <c r="C288">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>15</v>
+      </c>
+      <c r="B289">
+        <v>20200601</v>
+      </c>
+      <c r="C289">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>27</v>
+      </c>
+      <c r="B290">
+        <v>20200701</v>
+      </c>
+      <c r="C290">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>7</v>
+      </c>
+      <c r="B291">
+        <v>20200701</v>
+      </c>
+      <c r="C291">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>33</v>
+      </c>
+      <c r="B292">
+        <v>20200801</v>
+      </c>
+      <c r="C292">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>48</v>
+      </c>
+      <c r="B293">
+        <v>20200801</v>
+      </c>
+      <c r="C293">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>40</v>
+      </c>
+      <c r="B294">
+        <v>20200901</v>
+      </c>
+      <c r="C294">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>46</v>
+      </c>
+      <c r="B295">
+        <v>20200901</v>
+      </c>
+      <c r="C295">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>57</v>
+      </c>
+      <c r="B296">
+        <v>20201001</v>
+      </c>
+      <c r="C296">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>54</v>
+      </c>
+      <c r="B297">
+        <v>20201001</v>
+      </c>
+      <c r="C297">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>27</v>
+      </c>
+      <c r="B298">
+        <v>20201101</v>
+      </c>
+      <c r="C298">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>22</v>
+      </c>
+      <c r="B299">
+        <v>20201101</v>
+      </c>
+      <c r="C299">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>19</v>
+      </c>
+      <c r="B300">
         <v>20201201</v>
       </c>
-      <c r="C121">
+      <c r="C300">
         <v>396</v>
       </c>
     </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>43</v>
+      </c>
+      <c r="B301">
+        <v>20201201</v>
+      </c>
+      <c r="C301">
+        <v>705</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C301">
+    <sortCondition ref="B2:B301"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added dummy data for the other two fact tables
</commit_message>
<xml_diff>
--- a/Dummy Data/Fact_Customer_Metrics.xlsx
+++ b/Dummy Data/Fact_Customer_Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COLLEGE\BITS PILANI\SS 2nd Semester\DW\DW Project\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C7DE6B-A753-4557-89A8-FF69F37B0553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996612-25D6-45F8-B2A6-BE3AE1ADAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Customer ID</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Credit Score</t>
+  </si>
+  <si>
+    <t>Lineage Key</t>
   </si>
 </sst>
 </file>
@@ -351,18 +354,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="N198" sqref="N198"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,8 +376,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19</v>
       </c>
@@ -383,8 +390,11 @@
       <c r="C2">
         <v>698</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -394,8 +404,11 @@
       <c r="C3">
         <v>698</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>31</v>
       </c>
@@ -405,8 +418,11 @@
       <c r="C4">
         <v>788</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>32</v>
       </c>
@@ -416,8 +432,11 @@
       <c r="C5">
         <v>694</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -427,8 +446,11 @@
       <c r="C6">
         <v>694</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>36</v>
       </c>
@@ -438,8 +460,11 @@
       <c r="C7">
         <v>708</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -449,8 +474,11 @@
       <c r="C8">
         <v>730</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>51</v>
       </c>
@@ -460,8 +488,11 @@
       <c r="C9">
         <v>730</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>19</v>
       </c>
@@ -471,8 +502,11 @@
       <c r="C10">
         <v>700</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -482,8 +516,11 @@
       <c r="C11">
         <v>683</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>41</v>
       </c>
@@ -493,8 +530,11 @@
       <c r="C12">
         <v>683</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -504,8 +544,11 @@
       <c r="C13">
         <v>682</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>56</v>
       </c>
@@ -515,8 +558,11 @@
       <c r="C14">
         <v>709</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50</v>
       </c>
@@ -526,8 +572,11 @@
       <c r="C15">
         <v>709</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>38</v>
       </c>
@@ -537,8 +586,11 @@
       <c r="C16">
         <v>687</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -548,8 +600,11 @@
       <c r="C17">
         <v>815</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>59</v>
       </c>
@@ -559,8 +614,11 @@
       <c r="C18">
         <v>815</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>38</v>
       </c>
@@ -570,8 +628,11 @@
       <c r="C19">
         <v>848</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31</v>
       </c>
@@ -581,8 +642,11 @@
       <c r="C20">
         <v>323</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -592,8 +656,11 @@
       <c r="C21">
         <v>323</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -603,8 +670,11 @@
       <c r="C22">
         <v>786</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -614,8 +684,11 @@
       <c r="C23">
         <v>427</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -625,8 +698,11 @@
       <c r="C24">
         <v>427</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
@@ -636,8 +712,11 @@
       <c r="C25">
         <v>681</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16</v>
       </c>
@@ -647,8 +726,11 @@
       <c r="C26">
         <v>356</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>51</v>
       </c>
@@ -658,8 +740,11 @@
       <c r="C27">
         <v>356</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>29</v>
       </c>
@@ -669,8 +754,11 @@
       <c r="C28">
         <v>694</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>22</v>
       </c>
@@ -680,8 +768,11 @@
       <c r="C29">
         <v>696</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>35</v>
       </c>
@@ -691,8 +782,11 @@
       <c r="C30">
         <v>696</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
@@ -702,8 +796,11 @@
       <c r="C31">
         <v>680</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>40</v>
       </c>
@@ -713,8 +810,11 @@
       <c r="C32">
         <v>520</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>39</v>
       </c>
@@ -724,8 +824,11 @@
       <c r="C33">
         <v>520</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -735,8 +838,11 @@
       <c r="C34">
         <v>738</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -746,8 +852,11 @@
       <c r="C35">
         <v>766</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>45</v>
       </c>
@@ -757,8 +866,11 @@
       <c r="C36">
         <v>766</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>44</v>
       </c>
@@ -768,8 +880,11 @@
       <c r="C37">
         <v>709</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>48</v>
       </c>
@@ -779,8 +894,11 @@
       <c r="C38">
         <v>741</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>28</v>
       </c>
@@ -790,8 +908,11 @@
       <c r="C39">
         <v>741</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -801,8 +922,11 @@
       <c r="C40">
         <v>711</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>15</v>
       </c>
@@ -812,8 +936,11 @@
       <c r="C41">
         <v>785</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>32</v>
       </c>
@@ -823,8 +950,11 @@
       <c r="C42">
         <v>698</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>21</v>
       </c>
@@ -834,8 +964,11 @@
       <c r="C43">
         <v>304</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>39</v>
       </c>
@@ -845,8 +978,11 @@
       <c r="C44">
         <v>703</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>24</v>
       </c>
@@ -856,8 +992,11 @@
       <c r="C45">
         <v>694</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
@@ -867,8 +1006,11 @@
       <c r="C46">
         <v>856</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>57</v>
       </c>
@@ -878,8 +1020,11 @@
       <c r="C47">
         <v>711</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>18</v>
       </c>
@@ -889,8 +1034,11 @@
       <c r="C48">
         <v>730</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>14</v>
       </c>
@@ -900,8 +1048,11 @@
       <c r="C49">
         <v>606</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -911,8 +1062,11 @@
       <c r="C50">
         <v>706</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>11</v>
       </c>
@@ -922,8 +1076,11 @@
       <c r="C51">
         <v>683</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>46</v>
       </c>
@@ -933,8 +1090,11 @@
       <c r="C52">
         <v>789</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>22</v>
       </c>
@@ -944,8 +1104,11 @@
       <c r="C53">
         <v>737</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -955,8 +1118,11 @@
       <c r="C54">
         <v>709</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -966,8 +1132,11 @@
       <c r="C55">
         <v>759</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>51</v>
       </c>
@@ -977,8 +1146,11 @@
       <c r="C56">
         <v>753</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>31</v>
       </c>
@@ -988,8 +1160,11 @@
       <c r="C57">
         <v>815</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>60</v>
       </c>
@@ -999,8 +1174,11 @@
       <c r="C58">
         <v>731</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>43</v>
       </c>
@@ -1010,8 +1188,11 @@
       <c r="C59">
         <v>541</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1021,8 +1202,11 @@
       <c r="C60">
         <v>323</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>57</v>
       </c>
@@ -1032,8 +1216,11 @@
       <c r="C61">
         <v>796</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>23</v>
       </c>
@@ -1043,8 +1230,11 @@
       <c r="C62">
         <v>728</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>31</v>
       </c>
@@ -1054,8 +1244,11 @@
       <c r="C63">
         <v>427</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>35</v>
       </c>
@@ -1065,8 +1258,11 @@
       <c r="C64">
         <v>559</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>52</v>
       </c>
@@ -1076,8 +1272,11 @@
       <c r="C65">
         <v>680</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>28</v>
       </c>
@@ -1087,8 +1286,11 @@
       <c r="C66">
         <v>356</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>48</v>
       </c>
@@ -1098,8 +1300,11 @@
       <c r="C67">
         <v>721</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>44</v>
       </c>
@@ -1109,8 +1314,11 @@
       <c r="C68">
         <v>818</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>22</v>
       </c>
@@ -1120,8 +1328,11 @@
       <c r="C69">
         <v>696</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>54</v>
       </c>
@@ -1131,8 +1342,11 @@
       <c r="C70">
         <v>762</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>34</v>
       </c>
@@ -1142,8 +1356,11 @@
       <c r="C71">
         <v>690</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>34</v>
       </c>
@@ -1153,8 +1370,11 @@
       <c r="C72">
         <v>520</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5</v>
       </c>
@@ -1164,8 +1384,11 @@
       <c r="C73">
         <v>513</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -1175,8 +1398,11 @@
       <c r="C74">
         <v>674</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>51</v>
       </c>
@@ -1186,8 +1412,11 @@
       <c r="C75">
         <v>766</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15</v>
       </c>
@@ -1197,8 +1426,11 @@
       <c r="C76">
         <v>733</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>23</v>
       </c>
@@ -1208,8 +1440,11 @@
       <c r="C77">
         <v>714</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>38</v>
       </c>
@@ -1219,8 +1454,11 @@
       <c r="C78">
         <v>741</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>47</v>
       </c>
@@ -1230,8 +1468,11 @@
       <c r="C79">
         <v>735</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>58</v>
       </c>
@@ -1241,8 +1482,11 @@
       <c r="C80">
         <v>727</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>9</v>
       </c>
@@ -1252,8 +1496,11 @@
       <c r="C81">
         <v>785</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>55</v>
       </c>
@@ -1263,8 +1510,11 @@
       <c r="C82">
         <v>707</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>53</v>
       </c>
@@ -1274,8 +1524,11 @@
       <c r="C83">
         <v>310</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>16</v>
       </c>
@@ -1285,8 +1538,11 @@
       <c r="C84">
         <v>703</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>8</v>
       </c>
@@ -1296,8 +1552,11 @@
       <c r="C85">
         <v>845</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>12</v>
       </c>
@@ -1307,8 +1566,11 @@
       <c r="C86">
         <v>392</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>17</v>
       </c>
@@ -1318,8 +1580,11 @@
       <c r="C87">
         <v>711</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>58</v>
       </c>
@@ -1329,8 +1594,11 @@
       <c r="C88">
         <v>657</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>7</v>
       </c>
@@ -1340,8 +1608,11 @@
       <c r="C89">
         <v>716</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>42</v>
       </c>
@@ -1351,8 +1622,11 @@
       <c r="C90">
         <v>706</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>56</v>
       </c>
@@ -1362,8 +1636,11 @@
       <c r="C91">
         <v>703</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>49</v>
       </c>
@@ -1373,8 +1650,11 @@
       <c r="C92">
         <v>407</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>52</v>
       </c>
@@ -1384,8 +1664,11 @@
       <c r="C93">
         <v>737</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>53</v>
       </c>
@@ -1395,8 +1678,11 @@
       <c r="C94">
         <v>525</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7</v>
       </c>
@@ -1406,8 +1692,11 @@
       <c r="C95">
         <v>736</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>13</v>
       </c>
@@ -1417,8 +1706,11 @@
       <c r="C96">
         <v>753</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>25</v>
       </c>
@@ -1428,8 +1720,11 @@
       <c r="C97">
         <v>724</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>32</v>
       </c>
@@ -1439,8 +1734,11 @@
       <c r="C98">
         <v>696</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>35</v>
       </c>
@@ -1450,8 +1748,11 @@
       <c r="C99">
         <v>541</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>26</v>
       </c>
@@ -1461,8 +1762,11 @@
       <c r="C100">
         <v>721</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>55</v>
       </c>
@@ -1472,8 +1776,11 @@
       <c r="C101">
         <v>717</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20</v>
       </c>
@@ -1483,8 +1790,11 @@
       <c r="C102">
         <v>728</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>56</v>
       </c>
@@ -1494,8 +1804,11 @@
       <c r="C103">
         <v>534</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5</v>
       </c>
@@ -1505,8 +1818,11 @@
       <c r="C104">
         <v>799</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>11</v>
       </c>
@@ -1516,8 +1832,11 @@
       <c r="C105">
         <v>680</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>45</v>
       </c>
@@ -1527,8 +1846,11 @@
       <c r="C106">
         <v>684</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>23</v>
       </c>
@@ -1538,8 +1860,11 @@
       <c r="C107">
         <v>804</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>27</v>
       </c>
@@ -1549,8 +1874,11 @@
       <c r="C108">
         <v>818</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>36</v>
       </c>
@@ -1560,8 +1888,11 @@
       <c r="C109">
         <v>784</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>44</v>
       </c>
@@ -1571,8 +1902,11 @@
       <c r="C110">
         <v>736</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>13</v>
       </c>
@@ -1582,8 +1916,11 @@
       <c r="C111">
         <v>690</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>52</v>
       </c>
@@ -1593,8 +1930,11 @@
       <c r="C112">
         <v>723</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>29</v>
       </c>
@@ -1604,8 +1944,11 @@
       <c r="C113">
         <v>681</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>17</v>
       </c>
@@ -1615,8 +1958,11 @@
       <c r="C114">
         <v>674</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>15</v>
       </c>
@@ -1626,8 +1972,11 @@
       <c r="C115">
         <v>638</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>42</v>
       </c>
@@ -1637,8 +1986,11 @@
       <c r="C116">
         <v>355</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>58</v>
       </c>
@@ -1648,8 +2000,11 @@
       <c r="C117">
         <v>714</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>40</v>
       </c>
@@ -1659,8 +2014,11 @@
       <c r="C118">
         <v>751</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>48</v>
       </c>
@@ -1670,8 +2028,11 @@
       <c r="C119">
         <v>721</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>17</v>
       </c>
@@ -1681,8 +2042,11 @@
       <c r="C120">
         <v>727</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>36</v>
       </c>
@@ -1692,8 +2056,11 @@
       <c r="C121">
         <v>715</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>60</v>
       </c>
@@ -1703,8 +2070,11 @@
       <c r="C122">
         <v>735</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>8</v>
       </c>
@@ -1714,8 +2084,11 @@
       <c r="C123">
         <v>310</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>28</v>
       </c>
@@ -1725,8 +2098,11 @@
       <c r="C124">
         <v>688</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>13</v>
       </c>
@@ -1736,8 +2112,11 @@
       <c r="C125">
         <v>712</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>60</v>
       </c>
@@ -1747,8 +2126,11 @@
       <c r="C126">
         <v>392</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>33</v>
       </c>
@@ -1758,8 +2140,11 @@
       <c r="C127">
         <v>727</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>6</v>
       </c>
@@ -1769,8 +2154,11 @@
       <c r="C128">
         <v>885</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>26</v>
       </c>
@@ -1780,8 +2168,11 @@
       <c r="C129">
         <v>716</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>10</v>
       </c>
@@ -1791,8 +2182,11 @@
       <c r="C130">
         <v>726</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>38</v>
       </c>
@@ -1802,8 +2196,11 @@
       <c r="C131">
         <v>870</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>25</v>
       </c>
@@ -1813,8 +2210,11 @@
       <c r="C132">
         <v>407</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>59</v>
       </c>
@@ -1824,8 +2224,11 @@
       <c r="C133">
         <v>704</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>49</v>
       </c>
@@ -1835,8 +2238,11 @@
       <c r="C134">
         <v>443</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>47</v>
       </c>
@@ -1846,8 +2252,11 @@
       <c r="C135">
         <v>736</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>3</v>
       </c>
@@ -1857,8 +2266,11 @@
       <c r="C136">
         <v>723</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>4</v>
       </c>
@@ -1868,8 +2280,11 @@
       <c r="C137">
         <v>580</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1</v>
       </c>
@@ -1879,8 +2294,11 @@
       <c r="C138">
         <v>696</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>5</v>
       </c>
@@ -1890,8 +2308,11 @@
       <c r="C139">
         <v>638</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>55</v>
       </c>
@@ -1901,8 +2322,11 @@
       <c r="C140">
         <v>859</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>52</v>
       </c>
@@ -1912,8 +2336,11 @@
       <c r="C141">
         <v>717</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>22</v>
       </c>
@@ -1923,8 +2350,11 @@
       <c r="C142">
         <v>751</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>60</v>
       </c>
@@ -1934,8 +2364,11 @@
       <c r="C143">
         <v>713</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>47</v>
       </c>
@@ -1945,8 +2378,11 @@
       <c r="C144">
         <v>799</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2</v>
       </c>
@@ -1956,8 +2392,11 @@
       <c r="C145">
         <v>715</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>39</v>
       </c>
@@ -1967,8 +2406,11 @@
       <c r="C146">
         <v>733</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>12</v>
       </c>
@@ -1978,8 +2420,11 @@
       <c r="C147">
         <v>804</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>29</v>
       </c>
@@ -1989,8 +2434,11 @@
       <c r="C148">
         <v>688</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>50</v>
       </c>
@@ -2000,8 +2448,11 @@
       <c r="C149">
         <v>503</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>6</v>
       </c>
@@ -2011,8 +2462,11 @@
       <c r="C150">
         <v>736</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>45</v>
       </c>
@@ -2022,8 +2476,11 @@
       <c r="C151">
         <v>727</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>3</v>
       </c>
@@ -2033,8 +2490,11 @@
       <c r="C152">
         <v>699</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>59</v>
       </c>
@@ -2044,8 +2504,11 @@
       <c r="C153">
         <v>681</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>41</v>
       </c>
@@ -2055,8 +2518,11 @@
       <c r="C154">
         <v>726</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>25</v>
       </c>
@@ -2066,8 +2532,11 @@
       <c r="C155">
         <v>462</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>35</v>
       </c>
@@ -2077,8 +2546,11 @@
       <c r="C156">
         <v>355</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>56</v>
       </c>
@@ -2088,8 +2560,11 @@
       <c r="C157">
         <v>704</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>47</v>
       </c>
@@ -2099,8 +2574,11 @@
       <c r="C158">
         <v>744</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>18</v>
       </c>
@@ -2110,8 +2588,11 @@
       <c r="C159">
         <v>721</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>47</v>
       </c>
@@ -2121,8 +2602,11 @@
       <c r="C160">
         <v>883</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>43</v>
       </c>
@@ -2132,8 +2616,11 @@
       <c r="C161">
         <v>884</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>40</v>
       </c>
@@ -2143,8 +2630,11 @@
       <c r="C162">
         <v>735</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>12</v>
       </c>
@@ -2154,8 +2644,11 @@
       <c r="C163">
         <v>741</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>42</v>
       </c>
@@ -2165,8 +2658,11 @@
       <c r="C164">
         <v>723</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>39</v>
       </c>
@@ -2176,8 +2672,11 @@
       <c r="C165">
         <v>698</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>37</v>
       </c>
@@ -2187,8 +2686,11 @@
       <c r="C166">
         <v>703</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>19</v>
       </c>
@@ -2198,8 +2700,11 @@
       <c r="C167">
         <v>379</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>11</v>
       </c>
@@ -2209,8 +2714,11 @@
       <c r="C168">
         <v>694</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>10</v>
       </c>
@@ -2220,8 +2728,11 @@
       <c r="C169">
         <v>691</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>14</v>
       </c>
@@ -2231,8 +2742,11 @@
       <c r="C170">
         <v>722</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>31</v>
       </c>
@@ -2242,8 +2756,11 @@
       <c r="C171">
         <v>730</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>26</v>
       </c>
@@ -2253,8 +2770,11 @@
       <c r="C172">
         <v>688</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>28</v>
       </c>
@@ -2264,8 +2784,11 @@
       <c r="C173">
         <v>703</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>43</v>
       </c>
@@ -2275,8 +2798,11 @@
       <c r="C174">
         <v>683</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>55</v>
       </c>
@@ -2286,8 +2812,11 @@
       <c r="C175">
         <v>814</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>33</v>
       </c>
@@ -2297,8 +2826,11 @@
       <c r="C176">
         <v>696</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>6</v>
       </c>
@@ -2308,8 +2840,11 @@
       <c r="C177">
         <v>709</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1</v>
       </c>
@@ -2319,8 +2854,11 @@
       <c r="C178">
         <v>866</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>37</v>
       </c>
@@ -2330,8 +2868,11 @@
       <c r="C179">
         <v>456</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>49</v>
       </c>
@@ -2341,8 +2882,11 @@
       <c r="C180">
         <v>815</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>43</v>
       </c>
@@ -2352,8 +2896,11 @@
       <c r="C181">
         <v>471</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>16</v>
       </c>
@@ -2363,8 +2910,11 @@
       <c r="C182">
         <v>466</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>32</v>
       </c>
@@ -2374,8 +2924,11 @@
       <c r="C183">
         <v>323</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>44</v>
       </c>
@@ -2385,8 +2938,11 @@
       <c r="C184">
         <v>733</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>9</v>
       </c>
@@ -2396,8 +2952,11 @@
       <c r="C185">
         <v>427</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>21</v>
       </c>
@@ -2407,8 +2966,11 @@
       <c r="C186">
         <v>665</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>30</v>
       </c>
@@ -2418,8 +2980,11 @@
       <c r="C187">
         <v>356</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>58</v>
       </c>
@@ -2429,8 +2994,11 @@
       <c r="C188">
         <v>412</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>21</v>
       </c>
@@ -2440,8 +3008,11 @@
       <c r="C189">
         <v>696</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>2</v>
       </c>
@@ -2451,8 +3022,11 @@
       <c r="C190">
         <v>542</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>57</v>
       </c>
@@ -2462,8 +3036,11 @@
       <c r="C191">
         <v>520</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>29</v>
       </c>
@@ -2473,8 +3050,11 @@
       <c r="C192">
         <v>705</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>18</v>
       </c>
@@ -2484,8 +3064,11 @@
       <c r="C193">
         <v>766</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>49</v>
       </c>
@@ -2495,8 +3078,11 @@
       <c r="C194">
         <v>788</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>27</v>
       </c>
@@ -2506,8 +3092,11 @@
       <c r="C195">
         <v>741</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>24</v>
       </c>
@@ -2517,8 +3106,11 @@
       <c r="C196">
         <v>708</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>56</v>
       </c>
@@ -2528,8 +3120,11 @@
       <c r="C197">
         <v>785</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>32</v>
       </c>
@@ -2539,8 +3134,11 @@
       <c r="C198">
         <v>700</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>4</v>
       </c>
@@ -2550,8 +3148,11 @@
       <c r="C199">
         <v>703</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>58</v>
       </c>
@@ -2561,8 +3162,11 @@
       <c r="C200">
         <v>682</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>21</v>
       </c>
@@ -2572,8 +3176,11 @@
       <c r="C201">
         <v>711</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>12</v>
       </c>
@@ -2583,8 +3190,11 @@
       <c r="C202">
         <v>687</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>30</v>
       </c>
@@ -2594,8 +3204,11 @@
       <c r="C203">
         <v>706</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>5</v>
       </c>
@@ -2605,8 +3218,11 @@
       <c r="C204">
         <v>848</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>21</v>
       </c>
@@ -2616,8 +3232,11 @@
       <c r="C205">
         <v>737</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>57</v>
       </c>
@@ -2627,8 +3246,11 @@
       <c r="C206">
         <v>786</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>24</v>
       </c>
@@ -2638,8 +3260,11 @@
       <c r="C207">
         <v>753</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>3</v>
       </c>
@@ -2649,8 +3274,11 @@
       <c r="C208">
         <v>681</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>45</v>
       </c>
@@ -2660,8 +3288,11 @@
       <c r="C209">
         <v>541</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>34</v>
       </c>
@@ -2671,8 +3302,11 @@
       <c r="C210">
         <v>694</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D210">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>33</v>
       </c>
@@ -2682,8 +3316,11 @@
       <c r="C211">
         <v>728</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D211">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>36</v>
       </c>
@@ -2693,8 +3330,11 @@
       <c r="C212">
         <v>680</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D212">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>24</v>
       </c>
@@ -2704,8 +3344,11 @@
       <c r="C213">
         <v>680</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D213">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>29</v>
       </c>
@@ -2715,8 +3358,11 @@
       <c r="C214">
         <v>738</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D214">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>46</v>
       </c>
@@ -2726,8 +3372,11 @@
       <c r="C215">
         <v>818</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D215">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>49</v>
       </c>
@@ -2737,8 +3386,11 @@
       <c r="C216">
         <v>709</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>41</v>
       </c>
@@ -2748,8 +3400,11 @@
       <c r="C217">
         <v>690</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D217">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>4</v>
       </c>
@@ -2759,8 +3414,11 @@
       <c r="C218">
         <v>711</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D218">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>30</v>
       </c>
@@ -2770,8 +3428,11 @@
       <c r="C219">
         <v>674</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D219">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>25</v>
       </c>
@@ -2781,8 +3442,11 @@
       <c r="C220">
         <v>304</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D220">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>18</v>
       </c>
@@ -2792,8 +3456,11 @@
       <c r="C221">
         <v>714</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D221">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>3</v>
       </c>
@@ -2803,8 +3470,11 @@
       <c r="C222">
         <v>856</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D222">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>30</v>
       </c>
@@ -2814,8 +3484,11 @@
       <c r="C223">
         <v>727</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D223">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>14</v>
       </c>
@@ -2825,8 +3498,11 @@
       <c r="C224">
         <v>606</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D224">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>14</v>
       </c>
@@ -2836,8 +3512,11 @@
       <c r="C225">
         <v>310</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D225">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>50</v>
       </c>
@@ -2847,8 +3526,11 @@
       <c r="C226">
         <v>789</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D226">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>34</v>
       </c>
@@ -2858,8 +3540,11 @@
       <c r="C227">
         <v>392</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D227">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>51</v>
       </c>
@@ -2869,8 +3554,11 @@
       <c r="C228">
         <v>759</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D228">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>13</v>
       </c>
@@ -2880,8 +3568,11 @@
       <c r="C229">
         <v>716</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D229">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>20</v>
       </c>
@@ -2891,8 +3582,11 @@
       <c r="C230">
         <v>731</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D230">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>30</v>
       </c>
@@ -2902,8 +3596,11 @@
       <c r="C231">
         <v>407</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D231">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>54</v>
       </c>
@@ -2913,8 +3610,11 @@
       <c r="C232">
         <v>796</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D232">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>60</v>
       </c>
@@ -2924,8 +3624,11 @@
       <c r="C233">
         <v>736</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D233">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>6</v>
       </c>
@@ -2935,8 +3638,11 @@
       <c r="C234">
         <v>559</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D234">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>53</v>
       </c>
@@ -2946,8 +3652,11 @@
       <c r="C235">
         <v>696</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D235">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>8</v>
       </c>
@@ -2957,8 +3666,11 @@
       <c r="C236">
         <v>721</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D236">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>24</v>
       </c>
@@ -2968,8 +3680,11 @@
       <c r="C237">
         <v>717</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D237">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>16</v>
       </c>
@@ -2979,8 +3694,11 @@
       <c r="C238">
         <v>762</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D238">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>34</v>
       </c>
@@ -2990,8 +3708,11 @@
       <c r="C239">
         <v>799</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D239">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>41</v>
       </c>
@@ -3001,8 +3722,11 @@
       <c r="C240">
         <v>513</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D240">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>17</v>
       </c>
@@ -3012,8 +3736,11 @@
       <c r="C241">
         <v>804</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D241">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>45</v>
       </c>
@@ -3023,8 +3750,11 @@
       <c r="C242">
         <v>733</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D242">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>46</v>
       </c>
@@ -3034,8 +3764,11 @@
       <c r="C243">
         <v>736</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D243">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>5</v>
       </c>
@@ -3045,8 +3778,11 @@
       <c r="C244">
         <v>735</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D244">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>10</v>
       </c>
@@ -3056,8 +3792,11 @@
       <c r="C245">
         <v>681</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D245">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1</v>
       </c>
@@ -3067,8 +3806,11 @@
       <c r="C246">
         <v>707</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D246">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>36</v>
       </c>
@@ -3078,8 +3820,11 @@
       <c r="C247">
         <v>355</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D247">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>37</v>
       </c>
@@ -3089,8 +3834,11 @@
       <c r="C248">
         <v>845</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D248">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>33</v>
       </c>
@@ -3100,8 +3848,11 @@
       <c r="C249">
         <v>721</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D249">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>48</v>
       </c>
@@ -3111,8 +3862,11 @@
       <c r="C250">
         <v>657</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>50</v>
       </c>
@@ -3122,8 +3876,11 @@
       <c r="C251">
         <v>735</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D251">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>10</v>
       </c>
@@ -3133,8 +3890,11 @@
       <c r="C252">
         <v>703</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D252">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>46</v>
       </c>
@@ -3144,8 +3904,11 @@
       <c r="C253">
         <v>712</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D253">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>25</v>
       </c>
@@ -3155,8 +3918,11 @@
       <c r="C254">
         <v>525</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D254">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>15</v>
       </c>
@@ -3166,8 +3932,11 @@
       <c r="C255">
         <v>885</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D255">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>26</v>
       </c>
@@ -3177,8 +3946,11 @@
       <c r="C256">
         <v>724</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D256">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>2</v>
       </c>
@@ -3188,8 +3960,11 @@
       <c r="C257">
         <v>870</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>23</v>
       </c>
@@ -3199,8 +3974,11 @@
       <c r="C258">
         <v>721</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D258">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>38</v>
       </c>
@@ -3210,8 +3988,11 @@
       <c r="C259">
         <v>443</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D259">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>6</v>
       </c>
@@ -3221,8 +4002,11 @@
       <c r="C260">
         <v>534</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D260">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>17</v>
       </c>
@@ -3232,8 +4016,11 @@
       <c r="C261">
         <v>580</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D261">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>23</v>
       </c>
@@ -3243,8 +4030,11 @@
       <c r="C262">
         <v>684</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D262">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>9</v>
       </c>
@@ -3254,8 +4044,11 @@
       <c r="C263">
         <v>859</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D263">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>52</v>
       </c>
@@ -3265,8 +4058,11 @@
       <c r="C264">
         <v>784</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D264">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>54</v>
       </c>
@@ -3276,8 +4072,11 @@
       <c r="C265">
         <v>713</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D265">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>35</v>
       </c>
@@ -3287,8 +4086,11 @@
       <c r="C266">
         <v>723</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D266">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>42</v>
       </c>
@@ -3298,8 +4100,11 @@
       <c r="C267">
         <v>733</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D267">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>26</v>
       </c>
@@ -3309,8 +4114,11 @@
       <c r="C268">
         <v>638</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D268">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>54</v>
       </c>
@@ -3320,8 +4128,11 @@
       <c r="C269">
         <v>503</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D269">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>59</v>
       </c>
@@ -3331,8 +4142,11 @@
       <c r="C270">
         <v>751</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D270">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>12</v>
       </c>
@@ -3342,8 +4156,11 @@
       <c r="C271">
         <v>699</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D271">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>55</v>
       </c>
@@ -3353,8 +4170,11 @@
       <c r="C272">
         <v>715</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>39</v>
       </c>
@@ -3364,8 +4184,11 @@
       <c r="C273">
         <v>462</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>50</v>
       </c>
@@ -3375,8 +4198,11 @@
       <c r="C274">
         <v>688</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D274">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>44</v>
       </c>
@@ -3386,8 +4212,11 @@
       <c r="C275">
         <v>744</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D275">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>59</v>
       </c>
@@ -3397,8 +4226,11 @@
       <c r="C276">
         <v>727</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D276">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>16</v>
       </c>
@@ -3408,8 +4240,11 @@
       <c r="C277">
         <v>884</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D277">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1</v>
       </c>
@@ -3419,8 +4254,11 @@
       <c r="C278">
         <v>726</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D278">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>4</v>
       </c>
@@ -3430,8 +4268,11 @@
       <c r="C279">
         <v>723</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D279">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>53</v>
       </c>
@@ -3441,8 +4282,11 @@
       <c r="C280">
         <v>704</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D280">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>28</v>
       </c>
@@ -3452,8 +4296,11 @@
       <c r="C281">
         <v>379</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D281">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>37</v>
       </c>
@@ -3463,8 +4310,11 @@
       <c r="C282">
         <v>883</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D282">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>41</v>
       </c>
@@ -3474,8 +4324,11 @@
       <c r="C283">
         <v>722</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D283">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>37</v>
       </c>
@@ -3485,8 +4338,11 @@
       <c r="C284">
         <v>741</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D284">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>7</v>
       </c>
@@ -3496,8 +4352,11 @@
       <c r="C285">
         <v>703</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D285">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>20</v>
       </c>
@@ -3507,8 +4366,11 @@
       <c r="C286">
         <v>703</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D286">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>20</v>
       </c>
@@ -3518,8 +4380,11 @@
       <c r="C287">
         <v>696</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D287">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>27</v>
       </c>
@@ -3529,8 +4394,11 @@
       <c r="C288">
         <v>691</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>15</v>
       </c>
@@ -3540,8 +4408,11 @@
       <c r="C289">
         <v>456</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>27</v>
       </c>
@@ -3551,8 +4422,11 @@
       <c r="C290">
         <v>688</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>7</v>
       </c>
@@ -3562,8 +4436,11 @@
       <c r="C291">
         <v>466</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D291">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>33</v>
       </c>
@@ -3573,8 +4450,11 @@
       <c r="C292">
         <v>814</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D292">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>48</v>
       </c>
@@ -3584,8 +4464,11 @@
       <c r="C293">
         <v>733</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D293">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>40</v>
       </c>
@@ -3595,8 +4478,11 @@
       <c r="C294">
         <v>866</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D294">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>46</v>
       </c>
@@ -3606,8 +4492,11 @@
       <c r="C295">
         <v>665</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D295">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>57</v>
       </c>
@@ -3617,8 +4506,11 @@
       <c r="C296">
         <v>471</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D296">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>54</v>
       </c>
@@ -3628,8 +4520,11 @@
       <c r="C297">
         <v>412</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D297">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>27</v>
       </c>
@@ -3639,8 +4534,11 @@
       <c r="C298">
         <v>696</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D298">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>22</v>
       </c>
@@ -3650,8 +4548,11 @@
       <c r="C299">
         <v>542</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D299">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>19</v>
       </c>
@@ -3661,8 +4562,11 @@
       <c r="C300">
         <v>396</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D300">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>43</v>
       </c>
@@ -3671,6 +4575,9 @@
       </c>
       <c r="C301">
         <v>705</v>
+      </c>
+      <c r="D301">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Account_Metrics Fact table population script
</commit_message>
<xml_diff>
--- a/Dummy Data/Fact_Customer_Metrics.xlsx
+++ b/Dummy Data/Fact_Customer_Metrics.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COLLEGE\BITS PILANI\SS 2nd Semester\DW\DW Project\Loan-Data-Warehouse\Dummy Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem2\Data Warehousing\assigment\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996612-25D6-45F8-B2A6-BE3AE1ADAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC813A9-4AEB-4F7F-9531-A7C485543D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -354,19 +363,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D301"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,7 +389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>19</v>
       </c>
@@ -393,8 +402,12 @@
       <c r="D2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (19,20110101,698,8);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -407,8 +420,12 @@
       <c r="D3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (14,20110101,698,8);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>31</v>
       </c>
@@ -421,8 +438,12 @@
       <c r="D4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (31,20110101,788,8);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>32</v>
       </c>
@@ -435,8 +456,12 @@
       <c r="D5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (32,20110201,694,8);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -449,8 +474,12 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (10,20110201,694,8);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>36</v>
       </c>
@@ -463,8 +492,12 @@
       <c r="D7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (36,20110201,708,8);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
@@ -477,8 +510,12 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (11,20110301,730,8);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>51</v>
       </c>
@@ -491,8 +528,12 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (51,20110301,730,8);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>19</v>
       </c>
@@ -505,8 +546,12 @@
       <c r="D10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (19,20110301,700,8);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -519,8 +564,12 @@
       <c r="D11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (4,20110401,683,8);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>41</v>
       </c>
@@ -533,8 +582,12 @@
       <c r="D12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (41,20110401,683,8);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -547,8 +600,12 @@
       <c r="D13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (9,20110401,682,8);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>56</v>
       </c>
@@ -561,8 +618,12 @@
       <c r="D14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (56,20110501,709,8);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>50</v>
       </c>
@@ -575,8 +636,12 @@
       <c r="D15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (50,20110501,709,8);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>38</v>
       </c>
@@ -589,8 +654,12 @@
       <c r="D16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (38,20110501,687,8);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -603,8 +672,12 @@
       <c r="D17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (2,20110601,815,8);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>59</v>
       </c>
@@ -617,8 +690,12 @@
       <c r="D18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (59,20110601,815,8);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>38</v>
       </c>
@@ -631,8 +708,12 @@
       <c r="D19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (38,20110601,848,8);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>31</v>
       </c>
@@ -645,8 +726,12 @@
       <c r="D20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (31,20110701,323,8);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -659,8 +744,12 @@
       <c r="D21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (9,20110701,323,8);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>13</v>
       </c>
@@ -673,8 +762,12 @@
       <c r="D22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (13,20110701,786,8);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -687,8 +780,12 @@
       <c r="D23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (19,20110801,427,8);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -701,8 +798,12 @@
       <c r="D24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (20,20110801,427,8);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>18</v>
       </c>
@@ -715,8 +816,12 @@
       <c r="D25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (18,20110801,681,8);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -729,8 +834,12 @@
       <c r="D26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (16,20110901,356,8);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>51</v>
       </c>
@@ -743,8 +852,12 @@
       <c r="D27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (51,20110901,356,8);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>29</v>
       </c>
@@ -757,8 +870,12 @@
       <c r="D28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (29,20110901,694,8);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>22</v>
       </c>
@@ -771,8 +888,12 @@
       <c r="D29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (22,20111001,696,8);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>35</v>
       </c>
@@ -785,8 +906,12 @@
       <c r="D30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (35,20111001,696,8);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -799,8 +924,12 @@
       <c r="D31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (8,20111001,680,8);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>40</v>
       </c>
@@ -813,8 +942,12 @@
       <c r="D32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (40,20111101,520,8);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>39</v>
       </c>
@@ -827,8 +960,12 @@
       <c r="D33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (39,20111101,520,8);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>8</v>
       </c>
@@ -841,8 +978,12 @@
       <c r="D34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (8,20111101,738,8);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11</v>
       </c>
@@ -855,8 +996,12 @@
       <c r="D35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (11,20111201,766,8);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>45</v>
       </c>
@@ -869,8 +1014,12 @@
       <c r="D36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (45,20111201,766,8);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>44</v>
       </c>
@@ -883,8 +1032,12 @@
       <c r="D37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (44,20111201,709,8);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>48</v>
       </c>
@@ -897,8 +1050,12 @@
       <c r="D38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (48,20120101,741,8);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>28</v>
       </c>
@@ -911,8 +1068,12 @@
       <c r="D39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (28,20120101,741,8);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -925,8 +1086,12 @@
       <c r="D40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (40,20120101,711,8);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>15</v>
       </c>
@@ -939,8 +1104,12 @@
       <c r="D41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (15,20120201,785,8);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>32</v>
       </c>
@@ -953,8 +1122,12 @@
       <c r="D42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (32,20120201,698,8);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>21</v>
       </c>
@@ -967,8 +1140,12 @@
       <c r="D43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (21,20120201,304,8);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>39</v>
       </c>
@@ -981,8 +1158,12 @@
       <c r="D44">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (39,20120301,703,8);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>24</v>
       </c>
@@ -995,8 +1176,12 @@
       <c r="D45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (24,20120301,694,8);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>42</v>
       </c>
@@ -1009,8 +1194,12 @@
       <c r="D46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (42,20120301,856,8);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>57</v>
       </c>
@@ -1023,8 +1212,12 @@
       <c r="D47">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (57,20120401,711,8);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>18</v>
       </c>
@@ -1037,8 +1230,12 @@
       <c r="D48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (18,20120401,730,8);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>14</v>
       </c>
@@ -1051,8 +1248,12 @@
       <c r="D49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (14,20120401,606,8);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1065,8 +1266,12 @@
       <c r="D50">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (3,20120501,706,8);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>11</v>
       </c>
@@ -1079,8 +1284,12 @@
       <c r="D51">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (11,20120501,683,8);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>46</v>
       </c>
@@ -1093,8 +1302,12 @@
       <c r="D52">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (46,20120501,789,8);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>22</v>
       </c>
@@ -1107,8 +1320,12 @@
       <c r="D53">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (22,20120601,737,8);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1121,8 +1338,12 @@
       <c r="D54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (53,20120601,709,8);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1135,8 +1356,12 @@
       <c r="D55">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (7,20120601,759,8);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>51</v>
       </c>
@@ -1149,8 +1374,12 @@
       <c r="D56">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (51,20120701,753,8);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>31</v>
       </c>
@@ -1163,8 +1392,12 @@
       <c r="D57">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (31,20120701,815,8);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>60</v>
       </c>
@@ -1177,8 +1410,12 @@
       <c r="D58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (60,20120701,731,8);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>43</v>
       </c>
@@ -1191,8 +1428,12 @@
       <c r="D59">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (43,20120801,541,8);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1205,8 +1446,12 @@
       <c r="D60">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (1,20120801,323,8);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>57</v>
       </c>
@@ -1219,8 +1464,12 @@
       <c r="D61">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (57,20120801,796,8);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>23</v>
       </c>
@@ -1233,8 +1482,12 @@
       <c r="D62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (23,20120901,728,8);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>31</v>
       </c>
@@ -1247,8 +1500,12 @@
       <c r="D63">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (31,20120901,427,8);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>35</v>
       </c>
@@ -1261,8 +1518,12 @@
       <c r="D64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (35,20120901,559,8);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>52</v>
       </c>
@@ -1275,8 +1536,12 @@
       <c r="D65">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (52,20121001,680,8);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>28</v>
       </c>
@@ -1289,8 +1554,12 @@
       <c r="D66">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (28,20121001,356,8);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>48</v>
       </c>
@@ -1303,8 +1572,12 @@
       <c r="D67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F130" si="1">"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A67&amp;","&amp;B67&amp;","&amp;C67&amp;","&amp;D67&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (48,20121001,721,8);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>44</v>
       </c>
@@ -1317,8 +1590,12 @@
       <c r="D68">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (44,20121101,818,8);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>22</v>
       </c>
@@ -1331,8 +1608,12 @@
       <c r="D69">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (22,20121101,696,8);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>54</v>
       </c>
@@ -1345,8 +1626,12 @@
       <c r="D70">
         <v>8</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (54,20121101,762,8);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>34</v>
       </c>
@@ -1359,8 +1644,12 @@
       <c r="D71">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (34,20121201,690,8);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>34</v>
       </c>
@@ -1373,8 +1662,12 @@
       <c r="D72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (34,20121201,520,8);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>5</v>
       </c>
@@ -1387,8 +1680,12 @@
       <c r="D73">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (5,20121201,513,8);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2</v>
       </c>
@@ -1401,8 +1698,12 @@
       <c r="D74">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (2,20130101,674,8);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>51</v>
       </c>
@@ -1415,8 +1716,12 @@
       <c r="D75">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (51,20130101,766,8);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>15</v>
       </c>
@@ -1429,8 +1734,12 @@
       <c r="D76">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (15,20130101,733,8);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>23</v>
       </c>
@@ -1443,8 +1752,12 @@
       <c r="D77">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (23,20130201,714,8);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>38</v>
       </c>
@@ -1457,8 +1770,12 @@
       <c r="D78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (38,20130201,741,8);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>47</v>
       </c>
@@ -1471,8 +1788,12 @@
       <c r="D79">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (47,20130201,735,8);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>58</v>
       </c>
@@ -1485,8 +1806,12 @@
       <c r="D80">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (58,20130301,727,8);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>9</v>
       </c>
@@ -1499,8 +1824,12 @@
       <c r="D81">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (9,20130301,785,8);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>55</v>
       </c>
@@ -1513,8 +1842,12 @@
       <c r="D82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (55,20130301,707,8);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>53</v>
       </c>
@@ -1527,8 +1860,12 @@
       <c r="D83">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (53,20130401,310,8);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>16</v>
       </c>
@@ -1541,8 +1878,12 @@
       <c r="D84">
         <v>8</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (16,20130401,703,8);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8</v>
       </c>
@@ -1555,8 +1896,12 @@
       <c r="D85">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (8,20130401,845,8);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>12</v>
       </c>
@@ -1569,8 +1914,12 @@
       <c r="D86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (12,20130501,392,8);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>17</v>
       </c>
@@ -1583,8 +1932,12 @@
       <c r="D87">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F87" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (17,20130501,711,8);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>58</v>
       </c>
@@ -1597,8 +1950,12 @@
       <c r="D88">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F88" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (58,20130501,657,8);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>7</v>
       </c>
@@ -1611,8 +1968,12 @@
       <c r="D89">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F89" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (7,20130601,716,8);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>42</v>
       </c>
@@ -1625,8 +1986,12 @@
       <c r="D90">
         <v>8</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F90" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (42,20130601,706,8);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>56</v>
       </c>
@@ -1639,8 +2004,12 @@
       <c r="D91">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F91" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (56,20130601,703,8);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>49</v>
       </c>
@@ -1653,8 +2022,12 @@
       <c r="D92">
         <v>8</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F92" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (49,20130701,407,8);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>52</v>
       </c>
@@ -1667,8 +2040,12 @@
       <c r="D93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F93" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (52,20130701,737,8);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>53</v>
       </c>
@@ -1681,8 +2058,12 @@
       <c r="D94">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F94" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (53,20130701,525,8);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>7</v>
       </c>
@@ -1695,8 +2076,12 @@
       <c r="D95">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F95" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (7,20130801,736,8);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>13</v>
       </c>
@@ -1709,8 +2094,12 @@
       <c r="D96">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F96" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (13,20130801,753,8);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>25</v>
       </c>
@@ -1723,8 +2112,12 @@
       <c r="D97">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F97" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (25,20130801,724,8);</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>32</v>
       </c>
@@ -1737,8 +2130,12 @@
       <c r="D98">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F98" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (32,20130901,696,8);</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>35</v>
       </c>
@@ -1751,8 +2148,12 @@
       <c r="D99">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F99" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (35,20130901,541,8);</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>26</v>
       </c>
@@ -1765,8 +2166,12 @@
       <c r="D100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F100" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (26,20130901,721,8);</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>55</v>
       </c>
@@ -1779,8 +2184,12 @@
       <c r="D101">
         <v>8</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F101" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (55,20131001,717,8);</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>20</v>
       </c>
@@ -1793,8 +2202,12 @@
       <c r="D102">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F102" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (20,20131001,728,8);</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>56</v>
       </c>
@@ -1807,8 +2220,12 @@
       <c r="D103">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F103" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (56,20131001,534,8);</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>5</v>
       </c>
@@ -1821,8 +2238,12 @@
       <c r="D104">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F104" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (5,20131101,799,8);</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>11</v>
       </c>
@@ -1835,8 +2256,12 @@
       <c r="D105">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F105" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (11,20131101,680,8);</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>45</v>
       </c>
@@ -1849,8 +2274,12 @@
       <c r="D106">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F106" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (45,20131101,684,8);</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>23</v>
       </c>
@@ -1863,8 +2292,12 @@
       <c r="D107">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F107" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (23,20131201,804,8);</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>27</v>
       </c>
@@ -1877,8 +2310,12 @@
       <c r="D108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F108" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (27,20131201,818,8);</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>36</v>
       </c>
@@ -1891,8 +2328,12 @@
       <c r="D109">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F109" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (36,20131201,784,8);</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>44</v>
       </c>
@@ -1905,8 +2346,12 @@
       <c r="D110">
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F110" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (44,20140101,736,8);</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>13</v>
       </c>
@@ -1919,8 +2364,12 @@
       <c r="D111">
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F111" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (13,20140101,690,8);</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>52</v>
       </c>
@@ -1933,8 +2382,12 @@
       <c r="D112">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F112" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (52,20140101,723,8);</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>29</v>
       </c>
@@ -1947,8 +2400,12 @@
       <c r="D113">
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F113" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (29,20140201,681,8);</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>17</v>
       </c>
@@ -1961,8 +2418,12 @@
       <c r="D114">
         <v>8</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F114" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (17,20140201,674,8);</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>15</v>
       </c>
@@ -1975,8 +2436,12 @@
       <c r="D115">
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F115" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (15,20140201,638,8);</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>42</v>
       </c>
@@ -1989,8 +2454,12 @@
       <c r="D116">
         <v>8</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F116" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (42,20140301,355,8);</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>58</v>
       </c>
@@ -2003,8 +2472,12 @@
       <c r="D117">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F117" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (58,20140301,714,8);</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>40</v>
       </c>
@@ -2017,8 +2490,12 @@
       <c r="D118">
         <v>8</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F118" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (40,20140301,751,8);</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>48</v>
       </c>
@@ -2031,8 +2508,12 @@
       <c r="D119">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F119" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (48,20140401,721,8);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>17</v>
       </c>
@@ -2045,8 +2526,12 @@
       <c r="D120">
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F120" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (17,20140401,727,8);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>36</v>
       </c>
@@ -2059,8 +2544,12 @@
       <c r="D121">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F121" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (36,20140401,715,8);</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>60</v>
       </c>
@@ -2073,8 +2562,12 @@
       <c r="D122">
         <v>8</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F122" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (60,20140501,735,8);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>8</v>
       </c>
@@ -2087,8 +2580,12 @@
       <c r="D123">
         <v>8</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F123" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (8,20140501,310,8);</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>28</v>
       </c>
@@ -2101,8 +2598,12 @@
       <c r="D124">
         <v>8</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F124" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (28,20140501,688,8);</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>13</v>
       </c>
@@ -2115,8 +2616,12 @@
       <c r="D125">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F125" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (13,20140601,712,8);</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>60</v>
       </c>
@@ -2129,8 +2634,12 @@
       <c r="D126">
         <v>8</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F126" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (60,20140601,392,8);</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>33</v>
       </c>
@@ -2143,8 +2652,12 @@
       <c r="D127">
         <v>8</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F127" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (33,20140601,727,8);</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>6</v>
       </c>
@@ -2157,8 +2670,12 @@
       <c r="D128">
         <v>8</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F128" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (6,20140701,885,8);</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>26</v>
       </c>
@@ -2171,8 +2688,12 @@
       <c r="D129">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F129" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (26,20140701,716,8);</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>10</v>
       </c>
@@ -2185,8 +2706,12 @@
       <c r="D130">
         <v>8</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F130" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (10,20140701,726,8);</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>38</v>
       </c>
@@ -2199,8 +2724,12 @@
       <c r="D131">
         <v>8</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F131" t="str">
+        <f t="shared" ref="F131:F194" si="2">"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A131&amp;","&amp;B131&amp;","&amp;C131&amp;","&amp;D131&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (38,20140801,870,8);</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>25</v>
       </c>
@@ -2213,8 +2742,12 @@
       <c r="D132">
         <v>8</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F132" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (25,20140801,407,8);</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>59</v>
       </c>
@@ -2227,8 +2760,12 @@
       <c r="D133">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F133" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (59,20140801,704,8);</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>49</v>
       </c>
@@ -2241,8 +2778,12 @@
       <c r="D134">
         <v>8</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F134" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (49,20140901,443,8);</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>47</v>
       </c>
@@ -2255,8 +2796,12 @@
       <c r="D135">
         <v>8</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F135" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (47,20140901,736,8);</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>3</v>
       </c>
@@ -2269,8 +2814,12 @@
       <c r="D136">
         <v>8</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F136" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (3,20140901,723,8);</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>4</v>
       </c>
@@ -2283,8 +2832,12 @@
       <c r="D137">
         <v>8</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F137" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (4,20141001,580,8);</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1</v>
       </c>
@@ -2297,8 +2850,12 @@
       <c r="D138">
         <v>8</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F138" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (1,20141001,696,8);</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>5</v>
       </c>
@@ -2311,8 +2868,12 @@
       <c r="D139">
         <v>8</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F139" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (5,20141001,638,8);</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>55</v>
       </c>
@@ -2325,8 +2886,12 @@
       <c r="D140">
         <v>8</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F140" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (55,20141101,859,8);</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>52</v>
       </c>
@@ -2339,8 +2904,12 @@
       <c r="D141">
         <v>8</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F141" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (52,20141101,717,8);</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>22</v>
       </c>
@@ -2353,8 +2922,12 @@
       <c r="D142">
         <v>8</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F142" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (22,20141101,751,8);</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>60</v>
       </c>
@@ -2367,8 +2940,12 @@
       <c r="D143">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F143" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (60,20141201,713,8);</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>47</v>
       </c>
@@ -2381,8 +2958,12 @@
       <c r="D144">
         <v>8</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F144" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (47,20141201,799,8);</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2</v>
       </c>
@@ -2395,8 +2976,12 @@
       <c r="D145">
         <v>8</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F145" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (2,20141201,715,8);</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>39</v>
       </c>
@@ -2409,8 +2994,12 @@
       <c r="D146">
         <v>8</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F146" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (39,20150101,733,8);</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>12</v>
       </c>
@@ -2423,8 +3012,12 @@
       <c r="D147">
         <v>8</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F147" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (12,20150101,804,8);</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>29</v>
       </c>
@@ -2437,8 +3030,12 @@
       <c r="D148">
         <v>8</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F148" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (29,20150101,688,8);</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>50</v>
       </c>
@@ -2451,8 +3048,12 @@
       <c r="D149">
         <v>8</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F149" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (50,20150201,503,8);</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>6</v>
       </c>
@@ -2465,8 +3066,12 @@
       <c r="D150">
         <v>8</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F150" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (6,20150201,736,8);</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>45</v>
       </c>
@@ -2479,8 +3084,12 @@
       <c r="D151">
         <v>8</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F151" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (45,20150201,727,8);</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>3</v>
       </c>
@@ -2493,8 +3102,12 @@
       <c r="D152">
         <v>8</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F152" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (3,20150301,699,8);</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>59</v>
       </c>
@@ -2507,8 +3120,12 @@
       <c r="D153">
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F153" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (59,20150301,681,8);</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>41</v>
       </c>
@@ -2521,8 +3138,12 @@
       <c r="D154">
         <v>8</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F154" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (41,20150301,726,8);</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>25</v>
       </c>
@@ -2535,8 +3156,12 @@
       <c r="D155">
         <v>8</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F155" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (25,20150401,462,8);</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>35</v>
       </c>
@@ -2549,8 +3174,12 @@
       <c r="D156">
         <v>8</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F156" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (35,20150401,355,8);</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>56</v>
       </c>
@@ -2563,8 +3192,12 @@
       <c r="D157">
         <v>8</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F157" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (56,20150401,704,8);</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>47</v>
       </c>
@@ -2577,8 +3210,12 @@
       <c r="D158">
         <v>8</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F158" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (47,20150501,744,8);</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>18</v>
       </c>
@@ -2591,8 +3228,12 @@
       <c r="D159">
         <v>8</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F159" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (18,20150501,721,8);</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>47</v>
       </c>
@@ -2605,8 +3246,12 @@
       <c r="D160">
         <v>8</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F160" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (47,20150501,883,8);</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>43</v>
       </c>
@@ -2619,8 +3264,12 @@
       <c r="D161">
         <v>8</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F161" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (43,20150601,884,8);</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>40</v>
       </c>
@@ -2633,8 +3282,12 @@
       <c r="D162">
         <v>8</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F162" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (40,20150601,735,8);</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>12</v>
       </c>
@@ -2647,8 +3300,12 @@
       <c r="D163">
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F163" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (12,20150601,741,8);</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>42</v>
       </c>
@@ -2661,8 +3318,12 @@
       <c r="D164">
         <v>8</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F164" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (42,20150701,723,8);</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>39</v>
       </c>
@@ -2675,8 +3336,12 @@
       <c r="D165">
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F165" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (39,20150701,698,8);</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>37</v>
       </c>
@@ -2689,8 +3354,12 @@
       <c r="D166">
         <v>8</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F166" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (37,20150701,703,8);</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>19</v>
       </c>
@@ -2703,8 +3372,12 @@
       <c r="D167">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F167" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (19,20150801,379,8);</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>11</v>
       </c>
@@ -2717,8 +3390,12 @@
       <c r="D168">
         <v>8</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F168" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (11,20150801,694,8);</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>10</v>
       </c>
@@ -2731,8 +3408,12 @@
       <c r="D169">
         <v>8</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F169" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (10,20150801,691,8);</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>14</v>
       </c>
@@ -2745,8 +3426,12 @@
       <c r="D170">
         <v>8</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F170" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (14,20150901,722,8);</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>31</v>
       </c>
@@ -2759,8 +3444,12 @@
       <c r="D171">
         <v>8</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F171" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (31,20150901,730,8);</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>26</v>
       </c>
@@ -2773,8 +3462,12 @@
       <c r="D172">
         <v>8</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F172" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (26,20150901,688,8);</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>28</v>
       </c>
@@ -2787,8 +3480,12 @@
       <c r="D173">
         <v>8</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F173" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (28,20151001,703,8);</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>43</v>
       </c>
@@ -2801,8 +3498,12 @@
       <c r="D174">
         <v>8</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F174" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (43,20151001,683,8);</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>55</v>
       </c>
@@ -2815,8 +3516,12 @@
       <c r="D175">
         <v>8</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F175" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (55,20151001,814,8);</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>33</v>
       </c>
@@ -2829,8 +3534,12 @@
       <c r="D176">
         <v>8</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F176" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (33,20151101,696,8);</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>6</v>
       </c>
@@ -2843,8 +3552,12 @@
       <c r="D177">
         <v>8</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F177" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (6,20151101,709,8);</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1</v>
       </c>
@@ -2857,8 +3570,12 @@
       <c r="D178">
         <v>8</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F178" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (1,20151101,866,8);</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>37</v>
       </c>
@@ -2871,8 +3588,12 @@
       <c r="D179">
         <v>8</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F179" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (37,20151201,456,8);</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>49</v>
       </c>
@@ -2885,8 +3606,12 @@
       <c r="D180">
         <v>8</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F180" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (49,20151201,815,8);</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>43</v>
       </c>
@@ -2899,8 +3624,12 @@
       <c r="D181">
         <v>8</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F181" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (43,20151201,471,8);</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>16</v>
       </c>
@@ -2913,8 +3642,12 @@
       <c r="D182">
         <v>8</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F182" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (16,20160101,466,8);</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>32</v>
       </c>
@@ -2927,8 +3660,12 @@
       <c r="D183">
         <v>8</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F183" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (32,20160101,323,8);</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>44</v>
       </c>
@@ -2941,8 +3678,12 @@
       <c r="D184">
         <v>8</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F184" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (44,20160201,733,8);</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>9</v>
       </c>
@@ -2955,8 +3696,12 @@
       <c r="D185">
         <v>8</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F185" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (9,20160201,427,8);</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>21</v>
       </c>
@@ -2969,8 +3714,12 @@
       <c r="D186">
         <v>8</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F186" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (21,20160301,665,8);</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>30</v>
       </c>
@@ -2983,8 +3732,12 @@
       <c r="D187">
         <v>8</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F187" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (30,20160301,356,8);</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>58</v>
       </c>
@@ -2997,8 +3750,12 @@
       <c r="D188">
         <v>8</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F188" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (58,20160401,412,8);</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>21</v>
       </c>
@@ -3011,8 +3768,12 @@
       <c r="D189">
         <v>8</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F189" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (21,20160401,696,8);</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2</v>
       </c>
@@ -3025,8 +3786,12 @@
       <c r="D190">
         <v>8</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F190" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (2,20160501,542,8);</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>57</v>
       </c>
@@ -3039,8 +3804,12 @@
       <c r="D191">
         <v>8</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F191" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (57,20160501,520,8);</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>29</v>
       </c>
@@ -3053,8 +3822,12 @@
       <c r="D192">
         <v>8</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F192" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (29,20160601,705,8);</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>18</v>
       </c>
@@ -3067,8 +3840,12 @@
       <c r="D193">
         <v>8</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F193" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (18,20160601,766,8);</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>49</v>
       </c>
@@ -3081,8 +3858,12 @@
       <c r="D194">
         <v>8</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F194" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (49,20160701,788,8);</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>27</v>
       </c>
@@ -3095,8 +3876,12 @@
       <c r="D195">
         <v>8</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F195" t="str">
+        <f t="shared" ref="F195:F258" si="3">"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A195&amp;","&amp;B195&amp;","&amp;C195&amp;","&amp;D195&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (27,20160701,741,8);</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>24</v>
       </c>
@@ -3109,8 +3894,12 @@
       <c r="D196">
         <v>8</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F196" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (24,20160801,708,8);</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>56</v>
       </c>
@@ -3123,8 +3912,12 @@
       <c r="D197">
         <v>8</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F197" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (56,20160801,785,8);</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>32</v>
       </c>
@@ -3137,8 +3930,12 @@
       <c r="D198">
         <v>8</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F198" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (32,20160901,700,8);</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>4</v>
       </c>
@@ -3151,8 +3948,12 @@
       <c r="D199">
         <v>8</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F199" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (4,20160901,703,8);</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>58</v>
       </c>
@@ -3165,8 +3966,12 @@
       <c r="D200">
         <v>8</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F200" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (58,20161001,682,8);</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>21</v>
       </c>
@@ -3179,8 +3984,12 @@
       <c r="D201">
         <v>8</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F201" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (21,20161001,711,8);</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>12</v>
       </c>
@@ -3193,8 +4002,12 @@
       <c r="D202">
         <v>8</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F202" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (12,20161101,687,8);</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>30</v>
       </c>
@@ -3207,8 +4020,12 @@
       <c r="D203">
         <v>8</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F203" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (30,20161101,706,8);</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>5</v>
       </c>
@@ -3221,8 +4038,12 @@
       <c r="D204">
         <v>8</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F204" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (5,20161201,848,8);</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>21</v>
       </c>
@@ -3235,8 +4056,12 @@
       <c r="D205">
         <v>8</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F205" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (21,20161201,737,8);</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>57</v>
       </c>
@@ -3249,8 +4074,12 @@
       <c r="D206">
         <v>8</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F206" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (57,20170101,786,8);</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>24</v>
       </c>
@@ -3263,8 +4092,12 @@
       <c r="D207">
         <v>8</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F207" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (24,20170101,753,8);</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>3</v>
       </c>
@@ -3277,8 +4110,12 @@
       <c r="D208">
         <v>8</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F208" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (3,20170201,681,8);</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>45</v>
       </c>
@@ -3291,8 +4128,12 @@
       <c r="D209">
         <v>8</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F209" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (45,20170201,541,8);</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>34</v>
       </c>
@@ -3305,8 +4146,12 @@
       <c r="D210">
         <v>8</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F210" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (34,20170301,694,8);</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>33</v>
       </c>
@@ -3319,8 +4164,12 @@
       <c r="D211">
         <v>8</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F211" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (33,20170301,728,8);</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>36</v>
       </c>
@@ -3333,8 +4182,12 @@
       <c r="D212">
         <v>8</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F212" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (36,20170401,680,8);</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>24</v>
       </c>
@@ -3347,8 +4200,12 @@
       <c r="D213">
         <v>8</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F213" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (24,20170401,680,8);</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>29</v>
       </c>
@@ -3361,8 +4218,12 @@
       <c r="D214">
         <v>8</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F214" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (29,20170501,738,8);</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>46</v>
       </c>
@@ -3375,8 +4236,12 @@
       <c r="D215">
         <v>8</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F215" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (46,20170501,818,8);</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>49</v>
       </c>
@@ -3389,8 +4254,12 @@
       <c r="D216">
         <v>8</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F216" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (49,20170601,709,8);</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>41</v>
       </c>
@@ -3403,8 +4272,12 @@
       <c r="D217">
         <v>8</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F217" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (41,20170601,690,8);</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>4</v>
       </c>
@@ -3417,8 +4290,12 @@
       <c r="D218">
         <v>8</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F218" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (4,20170701,711,8);</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>30</v>
       </c>
@@ -3431,8 +4308,12 @@
       <c r="D219">
         <v>8</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F219" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (30,20170701,674,8);</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>25</v>
       </c>
@@ -3445,8 +4326,12 @@
       <c r="D220">
         <v>8</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F220" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (25,20170801,304,8);</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>18</v>
       </c>
@@ -3459,8 +4344,12 @@
       <c r="D221">
         <v>8</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F221" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (18,20170801,714,8);</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>3</v>
       </c>
@@ -3473,8 +4362,12 @@
       <c r="D222">
         <v>8</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F222" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (3,20170901,856,8);</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>30</v>
       </c>
@@ -3487,8 +4380,12 @@
       <c r="D223">
         <v>8</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F223" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (30,20170901,727,8);</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>14</v>
       </c>
@@ -3501,8 +4398,12 @@
       <c r="D224">
         <v>8</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F224" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (14,20171001,606,8);</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>14</v>
       </c>
@@ -3515,8 +4416,12 @@
       <c r="D225">
         <v>8</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F225" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (14,20171001,310,8);</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>50</v>
       </c>
@@ -3529,8 +4434,12 @@
       <c r="D226">
         <v>8</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F226" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (50,20171101,789,8);</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>34</v>
       </c>
@@ -3543,8 +4452,12 @@
       <c r="D227">
         <v>8</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F227" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (34,20171101,392,8);</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>51</v>
       </c>
@@ -3557,8 +4470,12 @@
       <c r="D228">
         <v>8</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F228" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (51,20171201,759,8);</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>13</v>
       </c>
@@ -3571,8 +4488,12 @@
       <c r="D229">
         <v>8</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F229" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (13,20171201,716,8);</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>20</v>
       </c>
@@ -3585,8 +4506,12 @@
       <c r="D230">
         <v>8</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F230" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (20,20180101,731,8);</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>30</v>
       </c>
@@ -3599,8 +4524,12 @@
       <c r="D231">
         <v>8</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F231" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (30,20180101,407,8);</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>54</v>
       </c>
@@ -3613,8 +4542,12 @@
       <c r="D232">
         <v>8</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F232" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (54,20180201,796,8);</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>60</v>
       </c>
@@ -3627,8 +4560,12 @@
       <c r="D233">
         <v>8</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F233" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (60,20180201,736,8);</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>6</v>
       </c>
@@ -3641,8 +4578,12 @@
       <c r="D234">
         <v>8</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F234" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (6,20180301,559,8);</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>53</v>
       </c>
@@ -3655,8 +4596,12 @@
       <c r="D235">
         <v>8</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F235" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (53,20180301,696,8);</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>8</v>
       </c>
@@ -3669,8 +4614,12 @@
       <c r="D236">
         <v>8</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F236" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (8,20180401,721,8);</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>24</v>
       </c>
@@ -3683,8 +4632,12 @@
       <c r="D237">
         <v>8</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F237" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (24,20180401,717,8);</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>16</v>
       </c>
@@ -3697,8 +4650,12 @@
       <c r="D238">
         <v>8</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F238" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (16,20180501,762,8);</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>34</v>
       </c>
@@ -3711,8 +4668,12 @@
       <c r="D239">
         <v>8</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F239" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (34,20180501,799,8);</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>41</v>
       </c>
@@ -3725,8 +4686,12 @@
       <c r="D240">
         <v>8</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F240" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (41,20180601,513,8);</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>17</v>
       </c>
@@ -3739,8 +4704,12 @@
       <c r="D241">
         <v>8</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F241" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (17,20180601,804,8);</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>45</v>
       </c>
@@ -3753,8 +4722,12 @@
       <c r="D242">
         <v>8</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F242" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (45,20180701,733,8);</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>46</v>
       </c>
@@ -3767,8 +4740,12 @@
       <c r="D243">
         <v>8</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F243" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (46,20180701,736,8);</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>5</v>
       </c>
@@ -3781,8 +4758,12 @@
       <c r="D244">
         <v>8</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F244" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (5,20180801,735,8);</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>10</v>
       </c>
@@ -3795,8 +4776,12 @@
       <c r="D245">
         <v>8</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F245" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (10,20180801,681,8);</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>1</v>
       </c>
@@ -3809,8 +4794,12 @@
       <c r="D246">
         <v>8</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F246" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (1,20180901,707,8);</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>36</v>
       </c>
@@ -3823,8 +4812,12 @@
       <c r="D247">
         <v>8</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F247" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (36,20180901,355,8);</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>37</v>
       </c>
@@ -3837,8 +4830,12 @@
       <c r="D248">
         <v>8</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F248" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (37,20181001,845,8);</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>33</v>
       </c>
@@ -3851,8 +4848,12 @@
       <c r="D249">
         <v>8</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F249" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (33,20181001,721,8);</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>48</v>
       </c>
@@ -3865,8 +4866,12 @@
       <c r="D250">
         <v>8</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F250" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (48,20181101,657,8);</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>50</v>
       </c>
@@ -3879,8 +4884,12 @@
       <c r="D251">
         <v>8</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F251" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (50,20181101,735,8);</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>10</v>
       </c>
@@ -3893,8 +4902,12 @@
       <c r="D252">
         <v>8</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F252" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (10,20181201,703,8);</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>46</v>
       </c>
@@ -3907,8 +4920,12 @@
       <c r="D253">
         <v>8</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F253" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (46,20181201,712,8);</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>25</v>
       </c>
@@ -3921,8 +4938,12 @@
       <c r="D254">
         <v>8</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F254" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (25,20190101,525,8);</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>15</v>
       </c>
@@ -3935,8 +4956,12 @@
       <c r="D255">
         <v>8</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F255" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (15,20190101,885,8);</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>26</v>
       </c>
@@ -3949,8 +4974,12 @@
       <c r="D256">
         <v>8</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F256" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (26,20190201,724,8);</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>2</v>
       </c>
@@ -3963,8 +4992,12 @@
       <c r="D257">
         <v>8</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F257" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (2,20190201,870,8);</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>23</v>
       </c>
@@ -3977,8 +5010,12 @@
       <c r="D258">
         <v>8</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F258" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (23,20190301,721,8);</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>38</v>
       </c>
@@ -3991,8 +5028,12 @@
       <c r="D259">
         <v>8</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F259" t="str">
+        <f t="shared" ref="F259:F301" si="4">"INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES ("&amp;A259&amp;","&amp;B259&amp;","&amp;C259&amp;","&amp;D259&amp;");"</f>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (38,20190301,443,8);</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>6</v>
       </c>
@@ -4005,8 +5046,12 @@
       <c r="D260">
         <v>8</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F260" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (6,20190401,534,8);</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>17</v>
       </c>
@@ -4019,8 +5064,12 @@
       <c r="D261">
         <v>8</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F261" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (17,20190401,580,8);</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>23</v>
       </c>
@@ -4033,8 +5082,12 @@
       <c r="D262">
         <v>8</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F262" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (23,20190501,684,8);</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>9</v>
       </c>
@@ -4047,8 +5100,12 @@
       <c r="D263">
         <v>8</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F263" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (9,20190501,859,8);</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>52</v>
       </c>
@@ -4061,8 +5118,12 @@
       <c r="D264">
         <v>8</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F264" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (52,20190601,784,8);</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>54</v>
       </c>
@@ -4075,8 +5136,12 @@
       <c r="D265">
         <v>8</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F265" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (54,20190601,713,8);</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>35</v>
       </c>
@@ -4089,8 +5154,12 @@
       <c r="D266">
         <v>8</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F266" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (35,20190701,723,8);</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>42</v>
       </c>
@@ -4103,8 +5172,12 @@
       <c r="D267">
         <v>8</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F267" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (42,20190701,733,8);</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>26</v>
       </c>
@@ -4117,8 +5190,12 @@
       <c r="D268">
         <v>8</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F268" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (26,20190801,638,8);</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>54</v>
       </c>
@@ -4131,8 +5208,12 @@
       <c r="D269">
         <v>8</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F269" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (54,20190801,503,8);</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>59</v>
       </c>
@@ -4145,8 +5226,12 @@
       <c r="D270">
         <v>8</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F270" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (59,20190901,751,8);</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>12</v>
       </c>
@@ -4159,8 +5244,12 @@
       <c r="D271">
         <v>8</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F271" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (12,20190901,699,8);</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>55</v>
       </c>
@@ -4173,8 +5262,12 @@
       <c r="D272">
         <v>8</v>
       </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F272" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (55,20191001,715,8);</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>39</v>
       </c>
@@ -4187,8 +5280,12 @@
       <c r="D273">
         <v>8</v>
       </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F273" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (39,20191001,462,8);</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>50</v>
       </c>
@@ -4201,8 +5298,12 @@
       <c r="D274">
         <v>8</v>
       </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F274" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (50,20191101,688,8);</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>44</v>
       </c>
@@ -4215,8 +5316,12 @@
       <c r="D275">
         <v>8</v>
       </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F275" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (44,20191101,744,8);</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>59</v>
       </c>
@@ -4229,8 +5334,12 @@
       <c r="D276">
         <v>8</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F276" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (59,20191201,727,8);</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>16</v>
       </c>
@@ -4243,8 +5352,12 @@
       <c r="D277">
         <v>8</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F277" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (16,20191201,884,8);</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>1</v>
       </c>
@@ -4257,8 +5370,12 @@
       <c r="D278">
         <v>8</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F278" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (1,20200101,726,8);</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>4</v>
       </c>
@@ -4271,8 +5388,12 @@
       <c r="D279">
         <v>8</v>
       </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F279" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (4,20200101,723,8);</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>53</v>
       </c>
@@ -4285,8 +5406,12 @@
       <c r="D280">
         <v>8</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F280" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (53,20200201,704,8);</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>28</v>
       </c>
@@ -4299,8 +5424,12 @@
       <c r="D281">
         <v>8</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F281" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (28,20200201,379,8);</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>37</v>
       </c>
@@ -4313,8 +5442,12 @@
       <c r="D282">
         <v>8</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F282" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (37,20200301,883,8);</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>41</v>
       </c>
@@ -4327,8 +5460,12 @@
       <c r="D283">
         <v>8</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F283" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (41,20200301,722,8);</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>37</v>
       </c>
@@ -4341,8 +5478,12 @@
       <c r="D284">
         <v>8</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F284" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (37,20200401,741,8);</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>7</v>
       </c>
@@ -4355,8 +5496,12 @@
       <c r="D285">
         <v>8</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F285" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (7,20200401,703,8);</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>20</v>
       </c>
@@ -4369,8 +5514,12 @@
       <c r="D286">
         <v>8</v>
       </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F286" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (20,20200501,703,8);</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>20</v>
       </c>
@@ -4383,8 +5532,12 @@
       <c r="D287">
         <v>8</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F287" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (20,20200501,696,8);</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>27</v>
       </c>
@@ -4397,8 +5550,12 @@
       <c r="D288">
         <v>8</v>
       </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F288" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (27,20200601,691,8);</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>15</v>
       </c>
@@ -4411,8 +5568,12 @@
       <c r="D289">
         <v>8</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F289" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (15,20200601,456,8);</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>27</v>
       </c>
@@ -4425,8 +5586,12 @@
       <c r="D290">
         <v>8</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F290" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (27,20200701,688,8);</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>7</v>
       </c>
@@ -4439,8 +5604,12 @@
       <c r="D291">
         <v>8</v>
       </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F291" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (7,20200701,466,8);</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>33</v>
       </c>
@@ -4453,8 +5622,12 @@
       <c r="D292">
         <v>8</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F292" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (33,20200801,814,8);</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>48</v>
       </c>
@@ -4467,8 +5640,12 @@
       <c r="D293">
         <v>8</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F293" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (48,20200801,733,8);</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>40</v>
       </c>
@@ -4481,8 +5658,12 @@
       <c r="D294">
         <v>8</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F294" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (40,20200901,866,8);</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>46</v>
       </c>
@@ -4495,8 +5676,12 @@
       <c r="D295">
         <v>8</v>
       </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F295" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (46,20200901,665,8);</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>57</v>
       </c>
@@ -4509,8 +5694,12 @@
       <c r="D296">
         <v>8</v>
       </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F296" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (57,20201001,471,8);</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>54</v>
       </c>
@@ -4523,8 +5712,12 @@
       <c r="D297">
         <v>8</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F297" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (54,20201001,412,8);</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>27</v>
       </c>
@@ -4537,8 +5730,12 @@
       <c r="D298">
         <v>8</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F298" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (27,20201101,696,8);</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>22</v>
       </c>
@@ -4551,8 +5748,12 @@
       <c r="D299">
         <v>8</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F299" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (22,20201101,542,8);</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>19</v>
       </c>
@@ -4565,8 +5766,12 @@
       <c r="D300">
         <v>8</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F300" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (19,20201201,396,8);</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>43</v>
       </c>
@@ -4578,6 +5783,10 @@
       </c>
       <c r="D301">
         <v>8</v>
+      </c>
+      <c r="F301" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT into [dbo].[Fact_Customer_Metrics] ([Customer Key], [Date Key],[Credit Score], [Lineage Key]) VALUES (43,20201201,705,8);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>